<commit_message>
first major program added for testing
Added Comp BS tables in order to test the database and make sure everything is doing what it is supposed to...didnt use ids in the excel in order to save readability
</commit_message>
<xml_diff>
--- a/db_schema.xlsx
+++ b/db_schema.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haydenlawler/Documents/Comp426/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brahm/Desktop/UNC notes/comp426/MajorPlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="126">
   <si>
     <t>Users</t>
   </si>
@@ -180,13 +180,238 @@
   </si>
   <si>
     <t xml:space="preserve">Foreign Key to Program </t>
+  </si>
+  <si>
+    <t>Comp 110</t>
+  </si>
+  <si>
+    <t>Comp 410</t>
+  </si>
+  <si>
+    <t>Comp 401</t>
+  </si>
+  <si>
+    <t>Comp 411</t>
+  </si>
+  <si>
+    <t>Programs</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Comp Sci BS</t>
+  </si>
+  <si>
+    <t>Comp Sci</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Comp</t>
+  </si>
+  <si>
+    <t>Comp 455</t>
+  </si>
+  <si>
+    <t>Comp 550</t>
+  </si>
+  <si>
+    <t>Math 547</t>
+  </si>
+  <si>
+    <t>Stor 435</t>
+  </si>
+  <si>
+    <t>Comp 283</t>
+  </si>
+  <si>
+    <t>Stor</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Program Requirements</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>1 of 2 Linear Courses</t>
+  </si>
+  <si>
+    <t>5 courses &gt;= 426</t>
+  </si>
+  <si>
+    <t>1 of 2 Discrete Courses</t>
+  </si>
+  <si>
+    <t>Math 231</t>
+  </si>
+  <si>
+    <t>Math 232</t>
+  </si>
+  <si>
+    <t>Math 233</t>
+  </si>
+  <si>
+    <t>1 of 2 Mechanics Courses</t>
+  </si>
+  <si>
+    <t>1 of 11 additional Science with Lab Courses</t>
+  </si>
+  <si>
+    <t>Courses in Program</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Program Req</t>
+  </si>
+  <si>
+    <t>Comp 116</t>
+  </si>
+  <si>
+    <t>1 of 2 Intro Comp class</t>
+  </si>
+  <si>
+    <t>1 of 2 intro Comp Class</t>
+  </si>
+  <si>
+    <t>Comp 426</t>
+  </si>
+  <si>
+    <t>Math 381</t>
+  </si>
+  <si>
+    <t>Math 577</t>
+  </si>
+  <si>
+    <t>Phys 116</t>
+  </si>
+  <si>
+    <t>Phys 118</t>
+  </si>
+  <si>
+    <t>Comp 541</t>
+  </si>
+  <si>
+    <t>Comp 521</t>
+  </si>
+  <si>
+    <t>Comp 431</t>
+  </si>
+  <si>
+    <t>Comp 530</t>
+  </si>
+  <si>
+    <t>Comp 435</t>
+  </si>
+  <si>
+    <t>Comp 433</t>
+  </si>
+  <si>
+    <t>Astr 101</t>
+  </si>
+  <si>
+    <t>Biol 101</t>
+  </si>
+  <si>
+    <t>Biol 202</t>
+  </si>
+  <si>
+    <t>Biol 205</t>
+  </si>
+  <si>
+    <t>Chem 101</t>
+  </si>
+  <si>
+    <t>Chem 102</t>
+  </si>
+  <si>
+    <t>Geol 101</t>
+  </si>
+  <si>
+    <t>Phys 117</t>
+  </si>
+  <si>
+    <t>Phys 119</t>
+  </si>
+  <si>
+    <t>Phys 351</t>
+  </si>
+  <si>
+    <t>Phys 352</t>
+  </si>
+  <si>
+    <t>Comp BS</t>
+  </si>
+  <si>
+    <t>Phys</t>
+  </si>
+  <si>
+    <t>Astr</t>
+  </si>
+  <si>
+    <t>Biol</t>
+  </si>
+  <si>
+    <t>Chem</t>
+  </si>
+  <si>
+    <t>Geol</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>prereq</t>
+  </si>
+  <si>
+    <t>Comp 110 or Comp 116</t>
+  </si>
+  <si>
+    <t>Math 110 and Math 130</t>
+  </si>
+  <si>
+    <t>Math 381 and Math 383</t>
+  </si>
+  <si>
+    <t>Comp 110 or Comp 401 and Comp 283 or Math 381</t>
+  </si>
+  <si>
+    <t>Comp 410 and Comp 283 or Math 381</t>
+  </si>
+  <si>
+    <t>Math 231 and Math 232</t>
+  </si>
+  <si>
+    <t>Math 231 or Math 232</t>
+  </si>
+  <si>
+    <t>Comp 410 and Comp 411</t>
+  </si>
+  <si>
+    <t>Math 232 and Phys 116</t>
+  </si>
+  <si>
+    <t>Math 232 and Phys 118</t>
+  </si>
+  <si>
+    <t>Math 233 and Phys 117 or Phys 119</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -215,6 +440,22 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -233,8 +474,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -243,7 +488,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -519,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:AN45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="88" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="AN33" sqref="AN33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,7 +783,7 @@
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -547,13 +796,22 @@
       <c r="D1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -566,32 +824,56 @@
       <c r="D3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -599,7 +881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -609,8 +891,11 @@
       <c r="C8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -620,13 +905,114 @@
       <c r="C9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" t="s">
+        <v>73</v>
+      </c>
+      <c r="L9" t="s">
+        <v>83</v>
+      </c>
+      <c r="M9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O9" t="s">
+        <v>54</v>
+      </c>
+      <c r="P9" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>75</v>
+      </c>
+      <c r="R9" t="s">
+        <v>76</v>
+      </c>
+      <c r="S9" t="s">
+        <v>77</v>
+      </c>
+      <c r="T9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -639,16 +1025,232 @@
       <c r="D13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P13" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>66</v>
+      </c>
+      <c r="R13" t="s">
+        <v>86</v>
+      </c>
+      <c r="S13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T13" t="s">
+        <v>87</v>
+      </c>
+      <c r="U13" t="s">
+        <v>88</v>
+      </c>
+      <c r="V13" t="s">
+        <v>89</v>
+      </c>
+      <c r="W13" t="s">
+        <v>85</v>
+      </c>
+      <c r="X13" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>103</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" t="s">
+        <v>62</v>
+      </c>
+      <c r="O14" t="s">
+        <v>63</v>
+      </c>
+      <c r="P14" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>73</v>
+      </c>
+      <c r="R14" t="s">
+        <v>73</v>
+      </c>
+      <c r="S14" t="s">
+        <v>71</v>
+      </c>
+      <c r="T14" t="s">
+        <v>71</v>
+      </c>
+      <c r="U14" t="s">
+        <v>77</v>
+      </c>
+      <c r="V14" t="s">
+        <v>77</v>
+      </c>
+      <c r="W14" t="s">
+        <v>72</v>
+      </c>
+      <c r="X14" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -656,7 +1258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -666,13 +1268,216 @@
       <c r="C16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" t="s">
+        <v>74</v>
+      </c>
+      <c r="L17" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" t="s">
+        <v>76</v>
+      </c>
+      <c r="N17" t="s">
+        <v>62</v>
+      </c>
+      <c r="O17" t="s">
+        <v>63</v>
+      </c>
+      <c r="P17" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>66</v>
+      </c>
+      <c r="R17" t="s">
+        <v>86</v>
+      </c>
+      <c r="S17" t="s">
+        <v>64</v>
+      </c>
+      <c r="T17" t="s">
+        <v>87</v>
+      </c>
+      <c r="U17" t="s">
+        <v>88</v>
+      </c>
+      <c r="V17" t="s">
+        <v>89</v>
+      </c>
+      <c r="W17" t="s">
+        <v>85</v>
+      </c>
+      <c r="X17" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>103</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" t="s">
+        <v>115</v>
+      </c>
+      <c r="I18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" t="s">
+        <v>116</v>
+      </c>
+      <c r="L18" t="s">
+        <v>74</v>
+      </c>
+      <c r="M18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N18" t="s">
+        <v>118</v>
+      </c>
+      <c r="O18" t="s">
+        <v>119</v>
+      </c>
+      <c r="P18" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>74</v>
+      </c>
+      <c r="R18" t="s">
+        <v>75</v>
+      </c>
+      <c r="S18" t="s">
+        <v>76</v>
+      </c>
+      <c r="T18" t="s">
+        <v>117</v>
+      </c>
+      <c r="U18" t="s">
+        <v>120</v>
+      </c>
+      <c r="V18" t="s">
+        <v>121</v>
+      </c>
+      <c r="W18" t="s">
+        <v>122</v>
+      </c>
+      <c r="X18" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>124</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -683,7 +1488,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -694,12 +1499,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -713,7 +1518,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -721,7 +1526,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -729,7 +1534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -737,7 +1542,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -745,12 +1550,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>5</v>
       </c>
@@ -763,37 +1571,469 @@
       <c r="D30" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" t="s">
+        <v>82</v>
+      </c>
+      <c r="H30" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" t="s">
+        <v>52</v>
+      </c>
+      <c r="J30" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" t="s">
+        <v>62</v>
+      </c>
+      <c r="L30" t="s">
+        <v>63</v>
+      </c>
+      <c r="M30" t="s">
+        <v>64</v>
+      </c>
+      <c r="N30" t="s">
+        <v>65</v>
+      </c>
+      <c r="O30" t="s">
+        <v>66</v>
+      </c>
+      <c r="P30" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>90</v>
+      </c>
+      <c r="R30" t="s">
+        <v>91</v>
+      </c>
+      <c r="S30" t="s">
+        <v>92</v>
+      </c>
+      <c r="T30" t="s">
+        <v>93</v>
+      </c>
+      <c r="U30" t="s">
+        <v>94</v>
+      </c>
+      <c r="V30" t="s">
+        <v>95</v>
+      </c>
+      <c r="W30" t="s">
+        <v>87</v>
+      </c>
+      <c r="X30" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>103</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="K31">
+        <v>3</v>
+      </c>
+      <c r="L31">
+        <v>3</v>
+      </c>
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="N31">
+        <v>3</v>
+      </c>
+      <c r="O31">
+        <v>3</v>
+      </c>
+      <c r="P31">
+        <v>3</v>
+      </c>
+      <c r="Q31">
+        <v>4</v>
+      </c>
+      <c r="R31">
+        <v>3</v>
+      </c>
+      <c r="S31">
+        <v>3</v>
+      </c>
+      <c r="T31">
+        <v>3</v>
+      </c>
+      <c r="U31">
+        <v>3</v>
+      </c>
+      <c r="V31">
+        <v>3</v>
+      </c>
+      <c r="W31">
+        <v>3</v>
+      </c>
+      <c r="X31">
+        <v>4</v>
+      </c>
+      <c r="Y31">
+        <v>4</v>
+      </c>
+      <c r="Z31">
+        <v>4</v>
+      </c>
+      <c r="AA31">
+        <v>3</v>
+      </c>
+      <c r="AB31">
+        <v>4</v>
+      </c>
+      <c r="AC31">
+        <v>4</v>
+      </c>
+      <c r="AD31">
+        <v>4</v>
+      </c>
+      <c r="AE31">
+        <v>4</v>
+      </c>
+      <c r="AF31">
+        <v>4</v>
+      </c>
+      <c r="AG31">
+        <v>4</v>
+      </c>
+      <c r="AH31">
+        <v>4</v>
+      </c>
+      <c r="AI31">
+        <v>4</v>
+      </c>
+      <c r="AJ31">
+        <v>4</v>
+      </c>
+      <c r="AK31">
+        <v>4</v>
+      </c>
+      <c r="AL31">
+        <v>4</v>
+      </c>
+      <c r="AM31">
+        <v>4</v>
+      </c>
+      <c r="AN31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
       <c r="B32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32">
+        <v>110</v>
+      </c>
+      <c r="G32">
+        <v>116</v>
+      </c>
+      <c r="H32">
+        <v>401</v>
+      </c>
+      <c r="I32">
+        <v>410</v>
+      </c>
+      <c r="J32">
+        <v>411</v>
+      </c>
+      <c r="K32">
+        <v>455</v>
+      </c>
+      <c r="L32">
+        <v>550</v>
+      </c>
+      <c r="M32">
+        <v>547</v>
+      </c>
+      <c r="N32">
+        <v>435</v>
+      </c>
+      <c r="O32">
+        <v>283</v>
+      </c>
+      <c r="P32">
+        <v>426</v>
+      </c>
+      <c r="Q32">
+        <v>541</v>
+      </c>
+      <c r="R32">
+        <v>521</v>
+      </c>
+      <c r="S32">
+        <v>431</v>
+      </c>
+      <c r="T32">
+        <v>530</v>
+      </c>
+      <c r="U32">
+        <v>435</v>
+      </c>
+      <c r="V32">
+        <v>433</v>
+      </c>
+      <c r="W32">
+        <v>577</v>
+      </c>
+      <c r="X32">
+        <v>231</v>
+      </c>
+      <c r="Y32">
+        <v>232</v>
+      </c>
+      <c r="Z32">
+        <v>233</v>
+      </c>
+      <c r="AA32">
+        <v>381</v>
+      </c>
+      <c r="AB32">
+        <v>116</v>
+      </c>
+      <c r="AC32">
+        <v>118</v>
+      </c>
+      <c r="AD32">
+        <v>101</v>
+      </c>
+      <c r="AE32">
+        <v>101</v>
+      </c>
+      <c r="AF32">
+        <v>202</v>
+      </c>
+      <c r="AG32">
+        <v>205</v>
+      </c>
+      <c r="AH32">
+        <v>101</v>
+      </c>
+      <c r="AI32">
+        <v>102</v>
+      </c>
+      <c r="AJ32">
+        <v>101</v>
+      </c>
+      <c r="AK32">
+        <v>117</v>
+      </c>
+      <c r="AL32">
+        <v>119</v>
+      </c>
+      <c r="AM32">
+        <v>351</v>
+      </c>
+      <c r="AN32">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="C33" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" t="s">
+        <v>61</v>
+      </c>
+      <c r="I33" t="s">
+        <v>61</v>
+      </c>
+      <c r="J33" t="s">
+        <v>61</v>
+      </c>
+      <c r="K33" t="s">
+        <v>61</v>
+      </c>
+      <c r="L33" t="s">
+        <v>61</v>
+      </c>
+      <c r="M33" t="s">
+        <v>68</v>
+      </c>
+      <c r="N33" t="s">
+        <v>67</v>
+      </c>
+      <c r="O33" t="s">
+        <v>61</v>
+      </c>
+      <c r="P33" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>61</v>
+      </c>
+      <c r="R33" t="s">
+        <v>61</v>
+      </c>
+      <c r="S33" t="s">
+        <v>61</v>
+      </c>
+      <c r="T33" t="s">
+        <v>61</v>
+      </c>
+      <c r="U33" t="s">
+        <v>61</v>
+      </c>
+      <c r="V33" t="s">
+        <v>61</v>
+      </c>
+      <c r="W33" t="s">
+        <v>68</v>
+      </c>
+      <c r="X33" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>16</v>
       </c>
@@ -804,7 +2044,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -815,12 +2055,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -834,7 +2074,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>27</v>
       </c>
@@ -848,12 +2088,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
@@ -864,7 +2104,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Added all courses and finished tables (hopefully all correct)
I did the Comp majors and minors, Math Ba, Econ BA, and math and stor minors so there are a total of 3 minor and 4 major programs...may have some logical things to deal with (such as how things are tagged).
</commit_message>
<xml_diff>
--- a/db_schema.xlsx
+++ b/db_schema.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="185">
   <si>
     <t>Users</t>
   </si>
@@ -405,13 +405,190 @@
   </si>
   <si>
     <t>Math 233 and Phys 117 or Phys 119</t>
+  </si>
+  <si>
+    <t>Comp BA</t>
+  </si>
+  <si>
+    <t>Comp Sci BA</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>Comp Minor</t>
+  </si>
+  <si>
+    <t>Comp Sci Minor</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>6 courses &gt;= 426 or Other Approved Electives</t>
+  </si>
+  <si>
+    <t>Maybe add BA and Minor Tags for these</t>
+  </si>
+  <si>
+    <t>2 courses &gt;= 426</t>
+  </si>
+  <si>
+    <t>Comp 590</t>
+  </si>
+  <si>
+    <t>Math 566</t>
+  </si>
+  <si>
+    <t>Phys 231</t>
+  </si>
+  <si>
+    <t>Math 383</t>
+  </si>
+  <si>
+    <t>Phys 114 or Phys 118</t>
+  </si>
+  <si>
+    <t>1 of 2 intro Stor Courses</t>
+  </si>
+  <si>
+    <t>Stor 155</t>
+  </si>
+  <si>
+    <t>Math 110</t>
+  </si>
+  <si>
+    <t>Econ</t>
+  </si>
+  <si>
+    <t>Math BA</t>
+  </si>
+  <si>
+    <t>Econ BA</t>
+  </si>
+  <si>
+    <t>Math Minor</t>
+  </si>
+  <si>
+    <t>Stats</t>
+  </si>
+  <si>
+    <t>Math 130</t>
+  </si>
+  <si>
+    <t>Math 528</t>
+  </si>
+  <si>
+    <t>Math Major</t>
+  </si>
+  <si>
+    <t>Math 529</t>
+  </si>
+  <si>
+    <t>Math 231 or Math 241</t>
+  </si>
+  <si>
+    <t>Math 232 or Math 283</t>
+  </si>
+  <si>
+    <t>Math 521</t>
+  </si>
+  <si>
+    <t>Math 524</t>
+  </si>
+  <si>
+    <t>3 Courses &gt;= 500</t>
+  </si>
+  <si>
+    <t>Math 241</t>
+  </si>
+  <si>
+    <t>Math 283</t>
+  </si>
+  <si>
+    <t>Math 533</t>
+  </si>
+  <si>
+    <t>Math 233 and Math 381</t>
+  </si>
+  <si>
+    <t>MATH 521</t>
+  </si>
+  <si>
+    <t>Econ 101</t>
+  </si>
+  <si>
+    <t>Econ 410</t>
+  </si>
+  <si>
+    <t>Econ 420</t>
+  </si>
+  <si>
+    <t>4 courses &gt;= 400</t>
+  </si>
+  <si>
+    <t>1 calculus from approved list</t>
+  </si>
+  <si>
+    <t>Stor 112</t>
+  </si>
+  <si>
+    <t>Econ 101 and Math 231 or Stor 112</t>
+  </si>
+  <si>
+    <t>Econ 400</t>
+  </si>
+  <si>
+    <t>Econ 423</t>
+  </si>
+  <si>
+    <t>Econ 511</t>
+  </si>
+  <si>
+    <t>Econ 545</t>
+  </si>
+  <si>
+    <t>Econ 560</t>
+  </si>
+  <si>
+    <t>Econ 410 and Math 233</t>
+  </si>
+  <si>
+    <t>Econ 445</t>
+  </si>
+  <si>
+    <t>Econ 460</t>
+  </si>
+  <si>
+    <t>Stor Minor</t>
+  </si>
+  <si>
+    <t>Stor 215 or Math 381</t>
+  </si>
+  <si>
+    <t>3 From approved list</t>
+  </si>
+  <si>
+    <t>Stor 215</t>
+  </si>
+  <si>
+    <t>Stor 305</t>
+  </si>
+  <si>
+    <t>Stor 415</t>
+  </si>
+  <si>
+    <t>Stor 445</t>
+  </si>
+  <si>
+    <t>Stor 455</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,6 +633,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -474,25 +658,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -768,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN45"/>
+  <dimension ref="A1:CL45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="88" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="AN33" sqref="AN33"/>
+    <sheetView tabSelected="1" topLeftCell="BD12" zoomScale="93" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="BT33" sqref="BT33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,7 +976,7 @@
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -800,7 +993,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -810,8 +1003,26 @@
       <c r="F2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" t="s">
+        <v>146</v>
+      </c>
+      <c r="K2" t="s">
+        <v>143</v>
+      </c>
+      <c r="L2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -830,8 +1041,26 @@
       <c r="F3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J3" t="s">
+        <v>146</v>
+      </c>
+      <c r="K3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -844,8 +1073,26 @@
       <c r="F4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -858,8 +1105,26 @@
       <c r="F5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I5" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K5" t="s">
+        <v>128</v>
+      </c>
+      <c r="L5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -870,10 +1135,28 @@
         <v>48</v>
       </c>
       <c r="F6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -881,7 +1164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -894,8 +1177,11 @@
       <c r="E8" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="U8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -953,8 +1239,119 @@
       <c r="T9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="U9" t="s">
+        <v>83</v>
+      </c>
+      <c r="V9" t="s">
+        <v>53</v>
+      </c>
+      <c r="W9" t="s">
+        <v>52</v>
+      </c>
+      <c r="X9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>134</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>152</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>154</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>156</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>156</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>152</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>162</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>169</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>163</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>141</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>141</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>178</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:90" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>24</v>
       </c>
@@ -1003,16 +1400,285 @@
       <c r="T10">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>6</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10">
+        <v>1</v>
+      </c>
+      <c r="AE10">
+        <v>1</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>6</v>
+      </c>
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
+        <v>1</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AM10">
+        <v>1</v>
+      </c>
+      <c r="AN10">
+        <v>1</v>
+      </c>
+      <c r="AO10">
+        <v>3</v>
+      </c>
+      <c r="AP10">
+        <v>1</v>
+      </c>
+      <c r="AQ10">
+        <v>1</v>
+      </c>
+      <c r="AR10">
+        <v>3</v>
+      </c>
+      <c r="AS10">
+        <v>1</v>
+      </c>
+      <c r="AT10">
+        <v>1</v>
+      </c>
+      <c r="AU10">
+        <v>1</v>
+      </c>
+      <c r="AV10">
+        <v>1</v>
+      </c>
+      <c r="AW10">
+        <v>1</v>
+      </c>
+      <c r="AX10">
+        <v>1</v>
+      </c>
+      <c r="AY10">
+        <v>1</v>
+      </c>
+      <c r="AZ10">
+        <v>4</v>
+      </c>
+      <c r="BA10">
+        <v>1</v>
+      </c>
+      <c r="BB10">
+        <v>1</v>
+      </c>
+      <c r="BC10">
+        <v>1</v>
+      </c>
+      <c r="BD10">
+        <v>1</v>
+      </c>
+      <c r="BE10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:90" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11" t="s">
+        <v>107</v>
+      </c>
+      <c r="K11" t="s">
+        <v>107</v>
+      </c>
+      <c r="L11" t="s">
+        <v>107</v>
+      </c>
+      <c r="M11" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" t="s">
+        <v>107</v>
+      </c>
+      <c r="O11" t="s">
+        <v>107</v>
+      </c>
+      <c r="P11" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>107</v>
+      </c>
+      <c r="R11" t="s">
+        <v>107</v>
+      </c>
+      <c r="S11" t="s">
+        <v>107</v>
+      </c>
+      <c r="T11" t="s">
+        <v>107</v>
+      </c>
+      <c r="U11" t="s">
+        <v>126</v>
+      </c>
+      <c r="V11" t="s">
+        <v>126</v>
+      </c>
+      <c r="W11" t="s">
+        <v>126</v>
+      </c>
+      <c r="X11" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>145</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>145</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>145</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>145</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>145</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>145</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>177</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>177</v>
+      </c>
+      <c r="BE11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1026,115 +1692,10 @@
         <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" t="s">
-        <v>52</v>
-      </c>
-      <c r="J13" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" t="s">
-        <v>74</v>
-      </c>
-      <c r="L13" t="s">
-        <v>75</v>
-      </c>
-      <c r="M13" t="s">
-        <v>76</v>
-      </c>
-      <c r="N13" t="s">
-        <v>62</v>
-      </c>
-      <c r="O13" t="s">
-        <v>63</v>
-      </c>
-      <c r="P13" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>66</v>
-      </c>
-      <c r="R13" t="s">
-        <v>86</v>
-      </c>
-      <c r="S13" t="s">
-        <v>64</v>
-      </c>
-      <c r="T13" t="s">
-        <v>87</v>
-      </c>
-      <c r="U13" t="s">
-        <v>88</v>
-      </c>
-      <c r="V13" t="s">
-        <v>89</v>
-      </c>
-      <c r="W13" t="s">
-        <v>85</v>
-      </c>
-      <c r="X13" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>98</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>100</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>101</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>103</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>104</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1142,13 +1703,13 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H14" t="s">
         <v>53</v>
@@ -1178,87 +1739,495 @@
         <v>65</v>
       </c>
       <c r="Q14" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="R14" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="S14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="T14" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="U14" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="V14" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="W14" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="X14" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="Y14" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="Z14" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="AA14" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="AB14" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="AC14" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="AD14" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="AE14" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="AF14" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="AG14" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="AH14" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="AI14" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="AJ14" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="AK14" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="AL14" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="AM14" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="AN14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>94</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>95</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>135</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>136</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>90</v>
+      </c>
+      <c r="BA14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>92</v>
+      </c>
+      <c r="BC14" t="s">
+        <v>93</v>
+      </c>
+      <c r="BD14" t="s">
+        <v>94</v>
+      </c>
+      <c r="BE14" t="s">
+        <v>95</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>141</v>
+      </c>
+      <c r="BG14" t="s">
+        <v>65</v>
+      </c>
+      <c r="BH14" t="s">
+        <v>155</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>149</v>
+      </c>
+      <c r="BJ14" t="s">
+        <v>151</v>
+      </c>
+      <c r="BK14" t="s">
+        <v>74</v>
+      </c>
+      <c r="BL14" t="s">
+        <v>157</v>
+      </c>
+      <c r="BM14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BN14" t="s">
+        <v>158</v>
+      </c>
+      <c r="BO14" t="s">
+        <v>86</v>
+      </c>
+      <c r="BP14" t="s">
+        <v>138</v>
+      </c>
+      <c r="BQ14" t="s">
+        <v>154</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>159</v>
+      </c>
+      <c r="BS14" t="s">
+        <v>162</v>
+      </c>
+      <c r="BT14" t="s">
+        <v>169</v>
+      </c>
+      <c r="BU14" t="s">
+        <v>163</v>
+      </c>
+      <c r="BV14" t="s">
+        <v>164</v>
+      </c>
+      <c r="BW14" t="s">
+        <v>141</v>
+      </c>
+      <c r="BX14" t="s">
+        <v>74</v>
+      </c>
+      <c r="BY14" t="s">
+        <v>167</v>
+      </c>
+      <c r="BZ14" t="s">
+        <v>170</v>
+      </c>
+      <c r="CA14" t="s">
+        <v>175</v>
+      </c>
+      <c r="CB14" t="s">
+        <v>171</v>
+      </c>
+      <c r="CC14" t="s">
+        <v>172</v>
+      </c>
+      <c r="CD14" t="s">
+        <v>173</v>
+      </c>
+      <c r="CE14" t="s">
+        <v>176</v>
+      </c>
+      <c r="CF14" t="s">
+        <v>180</v>
+      </c>
+      <c r="CG14" t="s">
+        <v>86</v>
+      </c>
+      <c r="CH14" t="s">
+        <v>181</v>
+      </c>
+      <c r="CI14" t="s">
+        <v>182</v>
+      </c>
+      <c r="CJ14" t="s">
+        <v>65</v>
+      </c>
+      <c r="CK14" t="s">
+        <v>183</v>
+      </c>
+      <c r="CL14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" t="s">
+        <v>74</v>
+      </c>
+      <c r="L15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N15" t="s">
+        <v>62</v>
+      </c>
+      <c r="O15" t="s">
+        <v>63</v>
+      </c>
+      <c r="P15" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>73</v>
+      </c>
+      <c r="R15" t="s">
+        <v>73</v>
+      </c>
+      <c r="S15" t="s">
+        <v>71</v>
+      </c>
+      <c r="T15" t="s">
+        <v>71</v>
+      </c>
+      <c r="U15" t="s">
+        <v>77</v>
+      </c>
+      <c r="V15" t="s">
+        <v>77</v>
+      </c>
+      <c r="W15" t="s">
+        <v>72</v>
+      </c>
+      <c r="X15" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>134</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>134</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>134</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>134</v>
+      </c>
+      <c r="BC15" t="s">
+        <v>134</v>
+      </c>
+      <c r="BD15" t="s">
+        <v>134</v>
+      </c>
+      <c r="BE15" t="s">
+        <v>134</v>
+      </c>
+      <c r="BF15" t="s">
+        <v>140</v>
+      </c>
+      <c r="BG15" t="s">
+        <v>140</v>
+      </c>
+      <c r="BH15" t="s">
+        <v>156</v>
+      </c>
+      <c r="BI15" t="s">
+        <v>156</v>
+      </c>
+      <c r="BJ15" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK15" t="s">
+        <v>152</v>
+      </c>
+      <c r="BL15" t="s">
+        <v>152</v>
+      </c>
+      <c r="BM15" t="s">
+        <v>153</v>
+      </c>
+      <c r="BN15" t="s">
+        <v>153</v>
+      </c>
+      <c r="BO15" t="s">
+        <v>86</v>
+      </c>
+      <c r="BP15" t="s">
+        <v>138</v>
+      </c>
+      <c r="BQ15" t="s">
+        <v>154</v>
+      </c>
+      <c r="BR15" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="BS15" t="s">
+        <v>162</v>
+      </c>
+      <c r="BT15" t="s">
+        <v>169</v>
+      </c>
+      <c r="BU15" t="s">
+        <v>163</v>
+      </c>
+      <c r="BV15" t="s">
+        <v>164</v>
+      </c>
+      <c r="BW15" t="s">
+        <v>141</v>
+      </c>
+      <c r="BX15" t="s">
+        <v>166</v>
+      </c>
+      <c r="BY15" t="s">
+        <v>166</v>
+      </c>
+      <c r="BZ15" t="s">
+        <v>165</v>
+      </c>
+      <c r="CA15" t="s">
+        <v>165</v>
+      </c>
+      <c r="CB15" t="s">
+        <v>165</v>
+      </c>
+      <c r="CC15" t="s">
+        <v>165</v>
+      </c>
+      <c r="CD15" t="s">
+        <v>165</v>
+      </c>
+      <c r="CE15" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="CF15" t="s">
+        <v>178</v>
+      </c>
+      <c r="CG15" t="s">
+        <v>178</v>
+      </c>
+      <c r="CH15" t="s">
+        <v>179</v>
+      </c>
+      <c r="CI15" t="s">
+        <v>179</v>
+      </c>
+      <c r="CJ15" t="s">
+        <v>179</v>
+      </c>
+      <c r="CK15" t="s">
+        <v>179</v>
+      </c>
+      <c r="CL15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1268,216 +2237,222 @@
       <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="17" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="E17" t="s">
-        <v>113</v>
-      </c>
-      <c r="F17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K17" t="s">
-        <v>74</v>
-      </c>
-      <c r="L17" t="s">
-        <v>75</v>
-      </c>
-      <c r="M17" t="s">
-        <v>76</v>
-      </c>
-      <c r="N17" t="s">
-        <v>62</v>
-      </c>
-      <c r="O17" t="s">
-        <v>63</v>
-      </c>
-      <c r="P17" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>66</v>
-      </c>
-      <c r="R17" t="s">
-        <v>86</v>
-      </c>
-      <c r="S17" t="s">
-        <v>64</v>
-      </c>
-      <c r="T17" t="s">
-        <v>87</v>
-      </c>
-      <c r="U17" t="s">
-        <v>88</v>
-      </c>
-      <c r="V17" t="s">
-        <v>89</v>
-      </c>
-      <c r="W17" t="s">
-        <v>85</v>
-      </c>
-      <c r="X17" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>98</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>99</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>100</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>101</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>102</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>103</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>104</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
       </c>
       <c r="H18" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="I18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K18" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="L18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N18" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
       <c r="O18" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="P18" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="Q18" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="R18" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="S18" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="T18" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="U18" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="V18" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="W18" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="X18" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="Y18" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="Z18" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="AA18" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="AB18" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="AC18" t="s">
-        <v>122</v>
+        <v>95</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>97</v>
       </c>
       <c r="AF18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AG18" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>100</v>
       </c>
       <c r="AI18" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>102</v>
       </c>
       <c r="AK18" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="AL18" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="AM18" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="AN18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="AO18" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>136</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>137</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>138</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>141</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>142</v>
+      </c>
+      <c r="AV18" t="s">
+        <v>148</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>155</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>149</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>151</v>
+      </c>
+      <c r="AZ18" t="s">
+        <v>157</v>
+      </c>
+      <c r="BA18" t="s">
+        <v>158</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>154</v>
+      </c>
+      <c r="BC18" t="s">
+        <v>159</v>
+      </c>
+      <c r="BD18" t="s">
+        <v>162</v>
+      </c>
+      <c r="BE18" t="s">
+        <v>169</v>
+      </c>
+      <c r="BF18" t="s">
+        <v>163</v>
+      </c>
+      <c r="BG18" t="s">
+        <v>164</v>
+      </c>
+      <c r="BH18" t="s">
+        <v>167</v>
+      </c>
+      <c r="BI18" t="s">
+        <v>170</v>
+      </c>
+      <c r="BJ18" t="s">
+        <v>175</v>
+      </c>
+      <c r="BK18" t="s">
+        <v>171</v>
+      </c>
+      <c r="BL18" t="s">
+        <v>172</v>
+      </c>
+      <c r="BM18" t="s">
+        <v>173</v>
+      </c>
+      <c r="BN18" t="s">
+        <v>176</v>
+      </c>
+      <c r="BO18" t="s">
+        <v>180</v>
+      </c>
+      <c r="BP18" t="s">
+        <v>181</v>
+      </c>
+      <c r="BQ18" t="s">
+        <v>182</v>
+      </c>
+      <c r="BR18" t="s">
+        <v>65</v>
+      </c>
+      <c r="BS18" t="s">
+        <v>183</v>
+      </c>
+      <c r="BT18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1487,8 +2462,185 @@
       <c r="C19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" t="s">
+        <v>115</v>
+      </c>
+      <c r="I19" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" t="s">
+        <v>116</v>
+      </c>
+      <c r="L19" t="s">
+        <v>74</v>
+      </c>
+      <c r="M19" t="s">
+        <v>75</v>
+      </c>
+      <c r="N19" t="s">
+        <v>118</v>
+      </c>
+      <c r="O19" t="s">
+        <v>119</v>
+      </c>
+      <c r="P19" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>74</v>
+      </c>
+      <c r="R19" t="s">
+        <v>75</v>
+      </c>
+      <c r="S19" t="s">
+        <v>76</v>
+      </c>
+      <c r="T19" t="s">
+        <v>117</v>
+      </c>
+      <c r="U19" t="s">
+        <v>120</v>
+      </c>
+      <c r="V19" t="s">
+        <v>121</v>
+      </c>
+      <c r="W19" t="s">
+        <v>122</v>
+      </c>
+      <c r="X19" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>124</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>105</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>138</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS19" t="s">
+        <v>142</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV19" t="s">
+        <v>142</v>
+      </c>
+      <c r="AW19" t="s">
+        <v>138</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>138</v>
+      </c>
+      <c r="AY19" t="s">
+        <v>138</v>
+      </c>
+      <c r="AZ19" t="s">
+        <v>148</v>
+      </c>
+      <c r="BA19" t="s">
+        <v>152</v>
+      </c>
+      <c r="BB19" t="s">
+        <v>160</v>
+      </c>
+      <c r="BC19" t="s">
+        <v>86</v>
+      </c>
+      <c r="BE19" t="s">
+        <v>162</v>
+      </c>
+      <c r="BF19" t="s">
+        <v>168</v>
+      </c>
+      <c r="BG19" t="s">
+        <v>163</v>
+      </c>
+      <c r="BH19" t="s">
+        <v>142</v>
+      </c>
+      <c r="BI19" t="s">
+        <v>164</v>
+      </c>
+      <c r="BJ19" t="s">
+        <v>163</v>
+      </c>
+      <c r="BK19" t="s">
+        <v>174</v>
+      </c>
+      <c r="BL19" t="s">
+        <v>175</v>
+      </c>
+      <c r="BM19" t="s">
+        <v>176</v>
+      </c>
+      <c r="BN19" t="s">
+        <v>163</v>
+      </c>
+      <c r="BO19" t="s">
+        <v>142</v>
+      </c>
+      <c r="BP19" t="s">
+        <v>141</v>
+      </c>
+      <c r="BQ19" t="s">
+        <v>64</v>
+      </c>
+      <c r="BR19" t="s">
+        <v>76</v>
+      </c>
+      <c r="BS19" t="s">
+        <v>65</v>
+      </c>
+      <c r="BT19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1499,12 +2651,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1518,7 +2670,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1526,7 +2678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1534,7 +2686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1542,7 +2694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1550,7 +2702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1558,7 +2710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>5</v>
       </c>
@@ -1679,8 +2831,104 @@
       <c r="AN30" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO30" t="s">
+        <v>142</v>
+      </c>
+      <c r="AP30" t="s">
+        <v>135</v>
+      </c>
+      <c r="AQ30" t="s">
+        <v>136</v>
+      </c>
+      <c r="AR30" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS30" t="s">
+        <v>138</v>
+      </c>
+      <c r="AT30" t="s">
+        <v>141</v>
+      </c>
+      <c r="AU30" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV30" t="s">
+        <v>148</v>
+      </c>
+      <c r="AW30" t="s">
+        <v>155</v>
+      </c>
+      <c r="AX30" t="s">
+        <v>149</v>
+      </c>
+      <c r="AY30" t="s">
+        <v>151</v>
+      </c>
+      <c r="AZ30" t="s">
+        <v>157</v>
+      </c>
+      <c r="BA30" t="s">
+        <v>158</v>
+      </c>
+      <c r="BB30" t="s">
+        <v>161</v>
+      </c>
+      <c r="BC30" t="s">
+        <v>159</v>
+      </c>
+      <c r="BD30" t="s">
+        <v>162</v>
+      </c>
+      <c r="BE30" t="s">
+        <v>169</v>
+      </c>
+      <c r="BF30" t="s">
+        <v>163</v>
+      </c>
+      <c r="BG30" t="s">
+        <v>164</v>
+      </c>
+      <c r="BH30" t="s">
+        <v>167</v>
+      </c>
+      <c r="BI30" t="s">
+        <v>170</v>
+      </c>
+      <c r="BJ30" t="s">
+        <v>175</v>
+      </c>
+      <c r="BK30" t="s">
+        <v>171</v>
+      </c>
+      <c r="BL30" t="s">
+        <v>172</v>
+      </c>
+      <c r="BM30" t="s">
+        <v>173</v>
+      </c>
+      <c r="BN30" t="s">
+        <v>176</v>
+      </c>
+      <c r="BO30" t="s">
+        <v>180</v>
+      </c>
+      <c r="BP30" t="s">
+        <v>181</v>
+      </c>
+      <c r="BQ30" t="s">
+        <v>182</v>
+      </c>
+      <c r="BR30" t="s">
+        <v>65</v>
+      </c>
+      <c r="BS30" t="s">
+        <v>183</v>
+      </c>
+      <c r="BT30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1795,8 +3043,104 @@
       <c r="AN31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO31">
+        <v>3</v>
+      </c>
+      <c r="AP31">
+        <v>3</v>
+      </c>
+      <c r="AQ31">
+        <v>3</v>
+      </c>
+      <c r="AR31">
+        <v>3</v>
+      </c>
+      <c r="AS31">
+        <v>3</v>
+      </c>
+      <c r="AT31">
+        <v>3</v>
+      </c>
+      <c r="AU31">
+        <v>3</v>
+      </c>
+      <c r="AV31">
+        <v>3</v>
+      </c>
+      <c r="AW31">
+        <v>3</v>
+      </c>
+      <c r="AX31">
+        <v>4</v>
+      </c>
+      <c r="AY31">
+        <v>4</v>
+      </c>
+      <c r="AZ31">
+        <v>4</v>
+      </c>
+      <c r="BA31">
+        <v>4</v>
+      </c>
+      <c r="BB31">
+        <v>3</v>
+      </c>
+      <c r="BC31">
+        <v>3</v>
+      </c>
+      <c r="BD31">
+        <v>3</v>
+      </c>
+      <c r="BE31">
+        <v>3</v>
+      </c>
+      <c r="BF31">
+        <v>3</v>
+      </c>
+      <c r="BG31">
+        <v>3</v>
+      </c>
+      <c r="BH31">
+        <v>3</v>
+      </c>
+      <c r="BI31">
+        <v>3</v>
+      </c>
+      <c r="BJ31">
+        <v>3</v>
+      </c>
+      <c r="BK31">
+        <v>3</v>
+      </c>
+      <c r="BL31">
+        <v>3</v>
+      </c>
+      <c r="BM31">
+        <v>3</v>
+      </c>
+      <c r="BN31">
+        <v>3</v>
+      </c>
+      <c r="BO31">
+        <v>3</v>
+      </c>
+      <c r="BP31">
+        <v>3</v>
+      </c>
+      <c r="BQ31">
+        <v>3</v>
+      </c>
+      <c r="BR31">
+        <v>3</v>
+      </c>
+      <c r="BS31">
+        <v>3</v>
+      </c>
+      <c r="BT31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1911,8 +3255,104 @@
       <c r="AN32">
         <v>352</v>
       </c>
-    </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO32">
+        <v>110</v>
+      </c>
+      <c r="AP32">
+        <v>590</v>
+      </c>
+      <c r="AQ32">
+        <v>566</v>
+      </c>
+      <c r="AR32">
+        <v>231</v>
+      </c>
+      <c r="AS32">
+        <v>383</v>
+      </c>
+      <c r="AT32">
+        <v>155</v>
+      </c>
+      <c r="AU32">
+        <v>435</v>
+      </c>
+      <c r="AV32">
+        <v>130</v>
+      </c>
+      <c r="AW32">
+        <v>524</v>
+      </c>
+      <c r="AX32">
+        <v>528</v>
+      </c>
+      <c r="AY32">
+        <v>529</v>
+      </c>
+      <c r="AZ32">
+        <v>241</v>
+      </c>
+      <c r="BA32">
+        <v>283</v>
+      </c>
+      <c r="BB32">
+        <v>521</v>
+      </c>
+      <c r="BC32">
+        <v>533</v>
+      </c>
+      <c r="BD32">
+        <v>101</v>
+      </c>
+      <c r="BE32">
+        <v>400</v>
+      </c>
+      <c r="BF32">
+        <v>410</v>
+      </c>
+      <c r="BG32">
+        <v>420</v>
+      </c>
+      <c r="BH32">
+        <v>112</v>
+      </c>
+      <c r="BI32">
+        <v>423</v>
+      </c>
+      <c r="BJ32">
+        <v>445</v>
+      </c>
+      <c r="BK32">
+        <v>511</v>
+      </c>
+      <c r="BL32">
+        <v>545</v>
+      </c>
+      <c r="BM32">
+        <v>560</v>
+      </c>
+      <c r="BN32">
+        <v>460</v>
+      </c>
+      <c r="BO32">
+        <v>215</v>
+      </c>
+      <c r="BP32">
+        <v>305</v>
+      </c>
+      <c r="BQ32">
+        <v>415</v>
+      </c>
+      <c r="BR32">
+        <v>435</v>
+      </c>
+      <c r="BS32">
+        <v>445</v>
+      </c>
+      <c r="BT32">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="33" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2027,13 +3467,109 @@
       <c r="AN33" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR33" t="s">
+        <v>108</v>
+      </c>
+      <c r="AS33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT33" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU33" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AY33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AZ33" t="s">
+        <v>68</v>
+      </c>
+      <c r="BA33" t="s">
+        <v>68</v>
+      </c>
+      <c r="BB33" t="s">
+        <v>68</v>
+      </c>
+      <c r="BC33" t="s">
+        <v>68</v>
+      </c>
+      <c r="BD33" t="s">
+        <v>143</v>
+      </c>
+      <c r="BE33" t="s">
+        <v>143</v>
+      </c>
+      <c r="BF33" t="s">
+        <v>143</v>
+      </c>
+      <c r="BG33" t="s">
+        <v>143</v>
+      </c>
+      <c r="BH33" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI33" t="s">
+        <v>143</v>
+      </c>
+      <c r="BJ33" t="s">
+        <v>143</v>
+      </c>
+      <c r="BK33" t="s">
+        <v>143</v>
+      </c>
+      <c r="BL33" t="s">
+        <v>143</v>
+      </c>
+      <c r="BM33" t="s">
+        <v>143</v>
+      </c>
+      <c r="BN33" t="s">
+        <v>143</v>
+      </c>
+      <c r="BO33" t="s">
+        <v>67</v>
+      </c>
+      <c r="BP33" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ33" t="s">
+        <v>67</v>
+      </c>
+      <c r="BR33" t="s">
+        <v>67</v>
+      </c>
+      <c r="BS33" t="s">
+        <v>67</v>
+      </c>
+      <c r="BT33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>16</v>
       </c>
@@ -2044,7 +3580,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -2055,12 +3591,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -2074,7 +3610,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>27</v>
       </c>
@@ -2088,12 +3624,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
@@ -2104,7 +3640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
fixed the prereq rows
should be good to go w handling ors and ands
</commit_message>
<xml_diff>
--- a/db_schema.xlsx
+++ b/db_schema.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haydenlawler/Documents/Comp426/MajorPlanner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brahm/Desktop/UNC notes/comp426/MajorPlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="184">
   <si>
     <t>Users</t>
   </si>
@@ -368,33 +368,6 @@
     <t>prereq</t>
   </si>
   <si>
-    <t>Comp 110 or Comp 116</t>
-  </si>
-  <si>
-    <t>Math 110 and Math 130</t>
-  </si>
-  <si>
-    <t>Math 381 and Math 383</t>
-  </si>
-  <si>
-    <t>Comp 110 or Comp 401 and Comp 283 or Math 381</t>
-  </si>
-  <si>
-    <t>Comp 410 and Comp 283 or Math 381</t>
-  </si>
-  <si>
-    <t>Math 231 and Math 232</t>
-  </si>
-  <si>
-    <t>Math 231 or Math 232</t>
-  </si>
-  <si>
-    <t>Comp 410 and Comp 411</t>
-  </si>
-  <si>
-    <t>Math 232 and Phys 116</t>
-  </si>
-  <si>
     <t>Math 232 and Phys 118</t>
   </si>
   <si>
@@ -500,9 +473,6 @@
     <t>Math 533</t>
   </si>
   <si>
-    <t>Math 233 and Math 381</t>
-  </si>
-  <si>
     <t>MATH 521</t>
   </si>
   <si>
@@ -524,9 +494,6 @@
     <t>Stor 112</t>
   </si>
   <si>
-    <t>Econ 101 and Math 231 or Stor 112</t>
-  </si>
-  <si>
     <t>Econ 400</t>
   </si>
   <si>
@@ -542,9 +509,6 @@
     <t>Econ 560</t>
   </si>
   <si>
-    <t>Econ 410 and Math 233</t>
-  </si>
-  <si>
     <t>Econ 445</t>
   </si>
   <si>
@@ -590,9 +554,6 @@
     <t>ECON</t>
   </si>
   <si>
-    <t>COMP ]</t>
-  </si>
-  <si>
     <t>Dept</t>
   </si>
   <si>
@@ -602,7 +563,22 @@
     <t>required</t>
   </si>
   <si>
-    <t>either intro comp class</t>
+    <t>either intro comp</t>
+  </si>
+  <si>
+    <t>1 discrete</t>
+  </si>
+  <si>
+    <t>1 of Mechanics</t>
+  </si>
+  <si>
+    <t>1 of Calc 1</t>
+  </si>
+  <si>
+    <t>Math 251</t>
+  </si>
+  <si>
+    <t>1 of Econ maths</t>
   </si>
 </sst>
 </file>
@@ -984,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CL46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:M6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="93" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="CJ20" sqref="CJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,22 +1019,22 @@
         <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="H3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="I3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="J3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="K3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="L3" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:90" x14ac:dyDescent="0.2">
@@ -1072,25 +1048,25 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="G4" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="H4" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="I4" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="J4" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="K4" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="L4" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:90" x14ac:dyDescent="0.2">
@@ -1107,22 +1083,22 @@
         <v>57</v>
       </c>
       <c r="G5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="H5" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="I5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="J5" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="K5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="L5" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:90" x14ac:dyDescent="0.2">
@@ -1179,7 +1155,7 @@
         <v>67</v>
       </c>
       <c r="U8" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:90" x14ac:dyDescent="0.2">
@@ -1253,7 +1229,7 @@
         <v>53</v>
       </c>
       <c r="Y9" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="Z9" t="s">
         <v>71</v>
@@ -1262,7 +1238,7 @@
         <v>72</v>
       </c>
       <c r="AB9" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="AC9" t="s">
         <v>81</v>
@@ -1277,13 +1253,13 @@
         <v>53</v>
       </c>
       <c r="AG9" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="AH9" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="AI9" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="AJ9" t="s">
         <v>74</v>
@@ -1292,64 +1268,64 @@
         <v>84</v>
       </c>
       <c r="AL9" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="AM9" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="AN9" t="s">
         <v>69</v>
       </c>
       <c r="AO9" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="AP9" t="s">
         <v>84</v>
       </c>
       <c r="AQ9" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="AR9" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="AS9" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="AT9" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="AU9" t="s">
         <v>74</v>
       </c>
       <c r="AV9" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="AW9" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="AX9" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="AY9" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="AZ9" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="BA9" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="BB9" t="s">
+        <v>153</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD9" t="s">
         <v>163</v>
       </c>
-      <c r="BC9" t="s">
-        <v>139</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>175</v>
-      </c>
       <c r="BE9" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:90" x14ac:dyDescent="0.2">
@@ -1563,115 +1539,115 @@
         <v>105</v>
       </c>
       <c r="U11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="V11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="W11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="X11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="Y11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="Z11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="AA11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="AB11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="AC11" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="AD11" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="AE11" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="AF11" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="AG11" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="AH11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="AI11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="AJ11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="AK11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="AL11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="AM11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="AN11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="AO11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="AP11" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="AQ11" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="AR11" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="AS11" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="AT11" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="AU11" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="AV11" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="AW11" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="AX11" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="AY11" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="AZ11" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="BA11" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="BB11" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="BC11" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="BD11" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="BE11" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:90" x14ac:dyDescent="0.2">
@@ -1833,13 +1809,13 @@
         <v>93</v>
       </c>
       <c r="AV14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="AW14" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="AX14" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="AY14" t="s">
         <v>83</v>
@@ -1863,103 +1839,103 @@
         <v>93</v>
       </c>
       <c r="BF14" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="BG14" t="s">
         <v>63</v>
       </c>
       <c r="BH14" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BI14" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="BJ14" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="BK14" t="s">
         <v>72</v>
       </c>
       <c r="BL14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="BM14" t="s">
         <v>73</v>
       </c>
       <c r="BN14" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="BO14" t="s">
         <v>84</v>
       </c>
       <c r="BP14" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="BQ14" t="s">
+        <v>142</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS14" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT14" t="s">
+        <v>155</v>
+      </c>
+      <c r="BU14" t="s">
+        <v>150</v>
+      </c>
+      <c r="BV14" t="s">
         <v>151</v>
       </c>
-      <c r="BR14" t="s">
-        <v>156</v>
-      </c>
-      <c r="BS14" t="s">
-        <v>159</v>
-      </c>
-      <c r="BT14" t="s">
-        <v>166</v>
-      </c>
-      <c r="BU14" t="s">
-        <v>160</v>
-      </c>
-      <c r="BV14" t="s">
-        <v>161</v>
-      </c>
       <c r="BW14" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="BX14" t="s">
         <v>72</v>
       </c>
       <c r="BY14" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="BZ14" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="CA14" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="CB14" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="CC14" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="CD14" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="CE14" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="CF14" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="CG14" t="s">
         <v>84</v>
       </c>
       <c r="CH14" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="CI14" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="CJ14" t="s">
         <v>63</v>
       </c>
       <c r="CK14" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="CL14" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:90" x14ac:dyDescent="0.2">
@@ -2078,173 +2054,173 @@
         <v>76</v>
       </c>
       <c r="AO15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AP15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AQ15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AR15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AS15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AT15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AU15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AV15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AW15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AX15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AY15" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="AZ15" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="BA15" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="BB15" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="BC15" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="BD15" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="BE15" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="BF15" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="BG15" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="BH15" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="BI15" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="BJ15" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="BK15" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="BL15" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="BM15" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="BN15" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="BO15" t="s">
         <v>84</v>
       </c>
       <c r="BP15" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="BQ15" t="s">
+        <v>142</v>
+      </c>
+      <c r="BR15" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="BS15" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT15" t="s">
+        <v>155</v>
+      </c>
+      <c r="BU15" t="s">
+        <v>150</v>
+      </c>
+      <c r="BV15" t="s">
         <v>151</v>
       </c>
-      <c r="BR15" s="5" t="s">
+      <c r="BW15" t="s">
+        <v>130</v>
+      </c>
+      <c r="BX15" t="s">
         <v>153</v>
       </c>
-      <c r="BS15" t="s">
-        <v>159</v>
-      </c>
-      <c r="BT15" t="s">
-        <v>166</v>
-      </c>
-      <c r="BU15" t="s">
-        <v>160</v>
-      </c>
-      <c r="BV15" t="s">
-        <v>161</v>
-      </c>
-      <c r="BW15" t="s">
-        <v>139</v>
-      </c>
-      <c r="BX15" t="s">
+      <c r="BY15" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CA15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CB15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CC15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CD15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CE15" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="CF15" t="s">
         <v>163</v>
       </c>
-      <c r="BY15" t="s">
+      <c r="CG15" t="s">
         <v>163</v>
       </c>
-      <c r="BZ15" t="s">
-        <v>162</v>
-      </c>
-      <c r="CA15" t="s">
-        <v>162</v>
-      </c>
-      <c r="CB15" t="s">
-        <v>162</v>
-      </c>
-      <c r="CC15" t="s">
-        <v>162</v>
-      </c>
-      <c r="CD15" t="s">
-        <v>162</v>
-      </c>
-      <c r="CE15" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="CF15" t="s">
-        <v>175</v>
-      </c>
-      <c r="CG15" t="s">
-        <v>175</v>
-      </c>
       <c r="CH15" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="CI15" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="CJ15" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="CK15" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="CL15" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:85" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -2252,211 +2228,248 @@
         <v>111</v>
       </c>
       <c r="F18" t="str">
-        <f>F30</f>
-        <v>Comp 110</v>
-      </c>
-      <c r="G18" t="str">
-        <f>G30</f>
-        <v>Comp 116</v>
-      </c>
-      <c r="H18" t="str">
         <f>H30</f>
         <v>Comp 401</v>
       </c>
+      <c r="G18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
       <c r="I18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J18" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="K18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M18" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="N18" t="s">
         <v>60</v>
       </c>
       <c r="O18" t="s">
+        <v>60</v>
+      </c>
+      <c r="P18" t="s">
         <v>61</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
+        <v>61</v>
+      </c>
+      <c r="R18" t="s">
+        <v>61</v>
+      </c>
+      <c r="S18" t="s">
         <v>63</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="T18" t="s">
         <v>64</v>
       </c>
-      <c r="R18" t="s">
+      <c r="U18" t="s">
         <v>84</v>
       </c>
-      <c r="S18" t="s">
+      <c r="V18" t="s">
         <v>62</v>
       </c>
-      <c r="T18" t="s">
+      <c r="W18" t="s">
         <v>85</v>
       </c>
-      <c r="U18" t="s">
+      <c r="X18" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y18" t="s">
         <v>86</v>
       </c>
-      <c r="V18" t="s">
+      <c r="Z18" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA18" t="s">
         <v>87</v>
       </c>
-      <c r="W18" t="s">
+      <c r="AB18" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC18" t="s">
         <v>83</v>
       </c>
-      <c r="X18" t="s">
+      <c r="AD18" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE18" t="s">
         <v>88</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="AF18" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG18" t="s">
         <v>89</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AH18" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI18" t="s">
         <v>90</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AJ18" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK18" t="s">
         <v>91</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AL18" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM18" t="s">
         <v>92</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AN18" t="s">
         <v>93</v>
       </c>
-      <c r="AD18" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>95</v>
-      </c>
-      <c r="AF18" t="s">
+      <c r="AO18" t="s">
         <v>96</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AP18" t="s">
         <v>97</v>
       </c>
-      <c r="AH18" t="s">
-        <v>98</v>
-      </c>
-      <c r="AI18" t="s">
+      <c r="AQ18" t="s">
         <v>99</v>
       </c>
-      <c r="AJ18" t="s">
-        <v>100</v>
-      </c>
-      <c r="AK18" t="s">
+      <c r="AR18" t="s">
         <v>101</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AS18" t="s">
+        <v>101</v>
+      </c>
+      <c r="AT18" t="s">
         <v>102</v>
       </c>
-      <c r="AM18" t="s">
+      <c r="AU18" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV18" t="s">
         <v>103</v>
       </c>
-      <c r="AN18" t="s">
+      <c r="AW18" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ18" t="s">
         <v>104</v>
       </c>
-      <c r="AO18" t="s">
-        <v>133</v>
-      </c>
-      <c r="AP18" t="s">
-        <v>134</v>
-      </c>
-      <c r="AQ18" t="s">
-        <v>135</v>
-      </c>
-      <c r="AR18" t="s">
+      <c r="BA18" t="s">
+        <v>125</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>127</v>
+      </c>
+      <c r="BC18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE18" t="s">
         <v>136</v>
       </c>
-      <c r="AS18" t="s">
+      <c r="BF18" t="s">
+        <v>143</v>
+      </c>
+      <c r="BG18" t="s">
+        <v>137</v>
+      </c>
+      <c r="BH18" t="s">
         <v>139</v>
       </c>
-      <c r="AT18" t="s">
+      <c r="BI18" t="s">
+        <v>145</v>
+      </c>
+      <c r="BJ18" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK18" t="s">
+        <v>146</v>
+      </c>
+      <c r="BL18" t="s">
+        <v>142</v>
+      </c>
+      <c r="BM18" t="s">
+        <v>182</v>
+      </c>
+      <c r="BN18" t="s">
+        <v>147</v>
+      </c>
+      <c r="BO18" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP18" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ18" t="s">
+        <v>150</v>
+      </c>
+      <c r="BR18" t="s">
+        <v>150</v>
+      </c>
+      <c r="BS18" t="s">
+        <v>151</v>
+      </c>
+      <c r="BT18" t="s">
+        <v>154</v>
+      </c>
+      <c r="BU18" t="s">
+        <v>156</v>
+      </c>
+      <c r="BV18" t="s">
+        <v>160</v>
+      </c>
+      <c r="BW18" t="s">
+        <v>157</v>
+      </c>
+      <c r="BX18" t="s">
+        <v>157</v>
+      </c>
+      <c r="BY18" t="s">
+        <v>158</v>
+      </c>
+      <c r="BZ18" t="s">
+        <v>159</v>
+      </c>
+      <c r="CA18" t="s">
+        <v>161</v>
+      </c>
+      <c r="CB18" t="s">
+        <v>165</v>
+      </c>
+      <c r="CC18" t="s">
+        <v>166</v>
+      </c>
+      <c r="CD18" t="s">
+        <v>167</v>
+      </c>
+      <c r="CE18" t="s">
         <v>63</v>
       </c>
-      <c r="AU18" t="s">
-        <v>140</v>
-      </c>
-      <c r="AV18" t="s">
-        <v>145</v>
-      </c>
-      <c r="AW18" t="s">
-        <v>152</v>
-      </c>
-      <c r="AX18" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY18" t="s">
-        <v>148</v>
-      </c>
-      <c r="AZ18" t="s">
-        <v>154</v>
-      </c>
-      <c r="BA18" t="s">
-        <v>155</v>
-      </c>
-      <c r="BB18" t="s">
-        <v>151</v>
-      </c>
-      <c r="BC18" t="s">
-        <v>156</v>
-      </c>
-      <c r="BD18" t="s">
-        <v>159</v>
-      </c>
-      <c r="BE18" t="s">
-        <v>166</v>
-      </c>
-      <c r="BF18" t="s">
-        <v>160</v>
-      </c>
-      <c r="BG18" t="s">
-        <v>161</v>
-      </c>
-      <c r="BH18" t="s">
-        <v>164</v>
-      </c>
-      <c r="BI18" t="s">
-        <v>167</v>
-      </c>
-      <c r="BJ18" t="s">
-        <v>172</v>
-      </c>
-      <c r="BK18" t="s">
+      <c r="CF18" t="s">
         <v>168</v>
       </c>
-      <c r="BL18" t="s">
+      <c r="CG18" t="s">
         <v>169</v>
       </c>
-      <c r="BM18" t="s">
-        <v>170</v>
-      </c>
-      <c r="BN18" t="s">
-        <v>173</v>
-      </c>
-      <c r="BO18" t="s">
-        <v>177</v>
-      </c>
-      <c r="BP18" t="s">
-        <v>178</v>
-      </c>
-      <c r="BQ18" t="s">
-        <v>179</v>
-      </c>
-      <c r="BR18" t="s">
-        <v>63</v>
-      </c>
-      <c r="BS18" t="s">
-        <v>180</v>
-      </c>
-      <c r="BT18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2469,185 +2482,248 @@
       <c r="E19" t="s">
         <v>112</v>
       </c>
+      <c r="F19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" t="s">
+        <v>80</v>
+      </c>
       <c r="H19" t="s">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="I19" t="s">
         <v>52</v>
       </c>
       <c r="J19" t="s">
+        <v>136</v>
+      </c>
+      <c r="K19" t="s">
+        <v>72</v>
+      </c>
+      <c r="L19" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19" t="s">
         <v>52</v>
       </c>
-      <c r="K19" t="s">
-        <v>114</v>
-      </c>
-      <c r="L19" t="s">
-        <v>72</v>
-      </c>
-      <c r="M19" t="s">
-        <v>73</v>
-      </c>
       <c r="N19" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="O19" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="P19" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="Q19" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="R19" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="S19" t="s">
         <v>74</v>
       </c>
       <c r="T19" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="U19" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="V19" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="W19" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="X19" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="Y19" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="Z19" t="s">
-        <v>120</v>
+        <v>73</v>
       </c>
       <c r="AA19" t="s">
-        <v>120</v>
+        <v>73</v>
       </c>
       <c r="AB19" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="AC19" t="s">
-        <v>120</v>
+        <v>53</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>53</v>
       </c>
       <c r="AF19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO19" t="s">
         <v>95</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AP19" t="s">
         <v>96</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AQ19" t="s">
         <v>98</v>
       </c>
-      <c r="AK19" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>122</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>123</v>
-      </c>
-      <c r="AN19" t="s">
+      <c r="AR19" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS19" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AW19" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>128</v>
+      </c>
+      <c r="AY19" t="s">
+        <v>87</v>
+      </c>
+      <c r="AZ19" t="s">
         <v>103</v>
       </c>
-      <c r="AP19" t="s">
+      <c r="BA19" t="s">
+        <v>127</v>
+      </c>
+      <c r="BB19" t="s">
+        <v>74</v>
+      </c>
+      <c r="BC19" t="s">
+        <v>131</v>
+      </c>
+      <c r="BD19" t="s">
+        <v>74</v>
+      </c>
+      <c r="BE19" t="s">
+        <v>131</v>
+      </c>
+      <c r="BF19" t="s">
+        <v>127</v>
+      </c>
+      <c r="BG19" t="s">
+        <v>127</v>
+      </c>
+      <c r="BH19" t="s">
+        <v>127</v>
+      </c>
+      <c r="BI19" t="s">
         <v>136</v>
       </c>
-      <c r="AQ19" t="s">
-        <v>137</v>
-      </c>
-      <c r="AR19" t="s">
+      <c r="BJ19" t="s">
+        <v>145</v>
+      </c>
+      <c r="BK19" t="s">
+        <v>72</v>
+      </c>
+      <c r="BL19" t="s">
         <v>74</v>
       </c>
-      <c r="AS19" t="s">
-        <v>140</v>
-      </c>
-      <c r="AT19" t="s">
+      <c r="BM19" t="s">
+        <v>84</v>
+      </c>
+      <c r="BN19" t="s">
+        <v>84</v>
+      </c>
+      <c r="BO19" t="s">
+        <v>149</v>
+      </c>
+      <c r="BP19" t="s">
+        <v>149</v>
+      </c>
+      <c r="BQ19" t="s">
+        <v>72</v>
+      </c>
+      <c r="BR19" t="s">
+        <v>154</v>
+      </c>
+      <c r="BS19" t="s">
+        <v>150</v>
+      </c>
+      <c r="BT19" t="s">
+        <v>131</v>
+      </c>
+      <c r="BU19" t="s">
+        <v>151</v>
+      </c>
+      <c r="BV19" t="s">
+        <v>150</v>
+      </c>
+      <c r="BW19" t="s">
+        <v>150</v>
+      </c>
+      <c r="BX19" t="s">
         <v>74</v>
       </c>
-      <c r="AV19" t="s">
-        <v>140</v>
-      </c>
-      <c r="AW19" t="s">
-        <v>136</v>
-      </c>
-      <c r="AX19" t="s">
-        <v>136</v>
-      </c>
-      <c r="AY19" t="s">
-        <v>136</v>
-      </c>
-      <c r="AZ19" t="s">
-        <v>145</v>
-      </c>
-      <c r="BA19" t="s">
-        <v>149</v>
-      </c>
-      <c r="BB19" t="s">
-        <v>157</v>
-      </c>
-      <c r="BC19" t="s">
-        <v>84</v>
-      </c>
-      <c r="BE19" t="s">
-        <v>159</v>
-      </c>
-      <c r="BF19" t="s">
-        <v>165</v>
-      </c>
-      <c r="BG19" t="s">
+      <c r="BY19" t="s">
         <v>160</v>
       </c>
-      <c r="BH19" t="s">
-        <v>140</v>
-      </c>
-      <c r="BI19" t="s">
+      <c r="BZ19" t="s">
         <v>161</v>
       </c>
-      <c r="BJ19" t="s">
-        <v>160</v>
-      </c>
-      <c r="BK19" t="s">
-        <v>171</v>
-      </c>
-      <c r="BL19" t="s">
-        <v>172</v>
-      </c>
-      <c r="BM19" t="s">
-        <v>173</v>
-      </c>
-      <c r="BN19" t="s">
-        <v>160</v>
-      </c>
-      <c r="BO19" t="s">
-        <v>140</v>
-      </c>
-      <c r="BP19" t="s">
-        <v>139</v>
-      </c>
-      <c r="BQ19" t="s">
+      <c r="CA19" t="s">
+        <v>150</v>
+      </c>
+      <c r="CB19" t="s">
+        <v>131</v>
+      </c>
+      <c r="CC19" t="s">
+        <v>130</v>
+      </c>
+      <c r="CD19" t="s">
         <v>62</v>
       </c>
-      <c r="BR19" t="s">
+      <c r="CE19" t="s">
         <v>74</v>
       </c>
-      <c r="BS19" t="s">
+      <c r="CF19" t="s">
         <v>63</v>
       </c>
-      <c r="BT19" t="s">
-        <v>139</v>
-      </c>
-      <c r="BU19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:73" x14ac:dyDescent="0.2">
+      <c r="CG19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2660,19 +2736,253 @@
       <c r="E20" t="s">
         <v>36</v>
       </c>
+      <c r="F20" t="s">
+        <v>178</v>
+      </c>
+      <c r="G20" t="s">
+        <v>178</v>
+      </c>
       <c r="H20" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="I20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="22" spans="1:73" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+      <c r="J20" t="s">
+        <v>177</v>
+      </c>
+      <c r="K20" t="s">
+        <v>177</v>
+      </c>
+      <c r="L20" t="s">
+        <v>177</v>
+      </c>
+      <c r="M20" t="s">
+        <v>177</v>
+      </c>
+      <c r="N20" t="s">
+        <v>179</v>
+      </c>
+      <c r="O20" t="s">
+        <v>179</v>
+      </c>
+      <c r="P20" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>179</v>
+      </c>
+      <c r="R20" t="s">
+        <v>179</v>
+      </c>
+      <c r="S20" t="s">
+        <v>177</v>
+      </c>
+      <c r="T20" t="s">
+        <v>177</v>
+      </c>
+      <c r="U20" t="s">
+        <v>177</v>
+      </c>
+      <c r="V20" t="s">
+        <v>177</v>
+      </c>
+      <c r="W20" t="s">
+        <v>177</v>
+      </c>
+      <c r="X20" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AW20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AX20" t="s">
+        <v>180</v>
+      </c>
+      <c r="AY20" t="s">
+        <v>180</v>
+      </c>
+      <c r="AZ20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BA20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BB20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BC20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BD20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BE20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BF20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BG20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BH20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BJ20" t="s">
+        <v>181</v>
+      </c>
+      <c r="BK20" t="s">
+        <v>181</v>
+      </c>
+      <c r="BL20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BM20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BN20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BO20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BP20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BQ20" t="s">
+        <v>183</v>
+      </c>
+      <c r="BR20" t="s">
+        <v>183</v>
+      </c>
+      <c r="BS20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BT20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BU20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BV20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BW20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BX20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BY20" t="s">
+        <v>177</v>
+      </c>
+      <c r="BZ20" t="s">
+        <v>177</v>
+      </c>
+      <c r="CA20" t="s">
+        <v>177</v>
+      </c>
+      <c r="CB20" t="s">
+        <v>177</v>
+      </c>
+      <c r="CC20" t="s">
+        <v>177</v>
+      </c>
+      <c r="CD20" t="s">
+        <v>177</v>
+      </c>
+      <c r="CE20" t="s">
+        <v>177</v>
+      </c>
+      <c r="CF20" t="s">
+        <v>177</v>
+      </c>
+      <c r="CG20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2686,7 +2996,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2694,7 +3004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2702,7 +3012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2710,7 +3020,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -2718,7 +3028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -2726,7 +3036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>5</v>
       </c>
@@ -2848,103 +3158,103 @@
         <v>104</v>
       </c>
       <c r="AO30" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="AP30" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="AQ30" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="AR30" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="AS30" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="AT30" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="AU30" t="s">
         <v>63</v>
       </c>
       <c r="AV30" t="s">
+        <v>136</v>
+      </c>
+      <c r="AW30" t="s">
+        <v>143</v>
+      </c>
+      <c r="AX30" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY30" t="s">
+        <v>139</v>
+      </c>
+      <c r="AZ30" t="s">
         <v>145</v>
       </c>
-      <c r="AW30" t="s">
-        <v>152</v>
-      </c>
-      <c r="AX30" t="s">
+      <c r="BA30" t="s">
         <v>146</v>
       </c>
-      <c r="AY30" t="s">
+      <c r="BB30" t="s">
         <v>148</v>
       </c>
-      <c r="AZ30" t="s">
+      <c r="BC30" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD30" t="s">
+        <v>149</v>
+      </c>
+      <c r="BE30" t="s">
+        <v>155</v>
+      </c>
+      <c r="BF30" t="s">
+        <v>150</v>
+      </c>
+      <c r="BG30" t="s">
+        <v>151</v>
+      </c>
+      <c r="BH30" t="s">
         <v>154</v>
       </c>
-      <c r="BA30" t="s">
-        <v>155</v>
-      </c>
-      <c r="BB30" t="s">
+      <c r="BI30" t="s">
+        <v>156</v>
+      </c>
+      <c r="BJ30" t="s">
+        <v>160</v>
+      </c>
+      <c r="BK30" t="s">
+        <v>157</v>
+      </c>
+      <c r="BL30" t="s">
         <v>158</v>
       </c>
-      <c r="BC30" t="s">
-        <v>156</v>
-      </c>
-      <c r="BD30" t="s">
+      <c r="BM30" t="s">
         <v>159</v>
       </c>
-      <c r="BE30" t="s">
+      <c r="BN30" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO30" t="s">
+        <v>165</v>
+      </c>
+      <c r="BP30" t="s">
         <v>166</v>
       </c>
-      <c r="BF30" t="s">
-        <v>160</v>
-      </c>
-      <c r="BG30" t="s">
-        <v>161</v>
-      </c>
-      <c r="BH30" t="s">
-        <v>164</v>
-      </c>
-      <c r="BI30" t="s">
+      <c r="BQ30" t="s">
         <v>167</v>
-      </c>
-      <c r="BJ30" t="s">
-        <v>172</v>
-      </c>
-      <c r="BK30" t="s">
-        <v>168</v>
-      </c>
-      <c r="BL30" t="s">
-        <v>169</v>
-      </c>
-      <c r="BM30" t="s">
-        <v>170</v>
-      </c>
-      <c r="BN30" t="s">
-        <v>173</v>
-      </c>
-      <c r="BO30" t="s">
-        <v>177</v>
-      </c>
-      <c r="BP30" t="s">
-        <v>178</v>
-      </c>
-      <c r="BQ30" t="s">
-        <v>179</v>
       </c>
       <c r="BR30" t="s">
         <v>63</v>
       </c>
       <c r="BS30" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="BT30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -3156,7 +3466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -3379,10 +3689,10 @@
         <v>18</v>
       </c>
       <c r="F33" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="G33" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="H33" t="s">
         <v>59</v>
@@ -3529,37 +3839,37 @@
         <v>66</v>
       </c>
       <c r="BD33" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="BE33" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="BF33" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="BG33" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="BH33" t="s">
         <v>65</v>
       </c>
       <c r="BI33" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="BJ33" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="BK33" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="BL33" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="BM33" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="BN33" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="BO33" t="s">
         <v>65</v>
@@ -3648,7 +3958,7 @@
         <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:72" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revised program requirements table
finished revising prog reqs
</commit_message>
<xml_diff>
--- a/db_schema.xlsx
+++ b/db_schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="184">
   <si>
     <t>Users</t>
   </si>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CL46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="93" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="CJ20" sqref="CJ20"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="93" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1172,16 +1172,16 @@
         <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>177</v>
       </c>
       <c r="H9" t="s">
         <v>69</v>
       </c>
       <c r="I9" t="s">
-        <v>63</v>
+        <v>177</v>
       </c>
       <c r="J9" t="s">
         <v>70</v>
@@ -1193,22 +1193,22 @@
         <v>81</v>
       </c>
       <c r="M9" t="s">
-        <v>52</v>
+        <v>177</v>
       </c>
       <c r="N9" t="s">
-        <v>51</v>
+        <v>177</v>
       </c>
       <c r="O9" t="s">
-        <v>53</v>
+        <v>177</v>
       </c>
       <c r="P9" t="s">
-        <v>72</v>
+        <v>177</v>
       </c>
       <c r="Q9" t="s">
-        <v>73</v>
+        <v>177</v>
       </c>
       <c r="R9" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="S9" t="s">
         <v>75</v>
@@ -1220,13 +1220,13 @@
         <v>81</v>
       </c>
       <c r="V9" t="s">
-        <v>52</v>
+        <v>177</v>
       </c>
       <c r="W9" t="s">
-        <v>51</v>
+        <v>177</v>
       </c>
       <c r="X9" t="s">
-        <v>53</v>
+        <v>177</v>
       </c>
       <c r="Y9" t="s">
         <v>121</v>
@@ -1235,7 +1235,7 @@
         <v>71</v>
       </c>
       <c r="AA9" t="s">
-        <v>72</v>
+        <v>177</v>
       </c>
       <c r="AB9" t="s">
         <v>129</v>
@@ -1244,13 +1244,13 @@
         <v>81</v>
       </c>
       <c r="AD9" t="s">
-        <v>52</v>
+        <v>177</v>
       </c>
       <c r="AE9" t="s">
-        <v>51</v>
+        <v>177</v>
       </c>
       <c r="AF9" t="s">
-        <v>53</v>
+        <v>177</v>
       </c>
       <c r="AG9" t="s">
         <v>123</v>
@@ -1262,16 +1262,16 @@
         <v>141</v>
       </c>
       <c r="AJ9" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="AK9" t="s">
-        <v>84</v>
+        <v>177</v>
       </c>
       <c r="AL9" t="s">
-        <v>127</v>
+        <v>177</v>
       </c>
       <c r="AM9" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="AN9" t="s">
         <v>69</v>
@@ -1280,10 +1280,10 @@
         <v>144</v>
       </c>
       <c r="AP9" t="s">
-        <v>84</v>
+        <v>177</v>
       </c>
       <c r="AQ9" t="s">
-        <v>127</v>
+        <v>177</v>
       </c>
       <c r="AR9" t="s">
         <v>144</v>
@@ -1295,31 +1295,31 @@
         <v>141</v>
       </c>
       <c r="AU9" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="AV9" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="AW9" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="AX9" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="AY9" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="AZ9" t="s">
         <v>152</v>
       </c>
       <c r="BA9" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="BB9" t="s">
         <v>153</v>
       </c>
       <c r="BC9" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="BD9" t="s">
         <v>163</v>
@@ -1654,6 +1654,162 @@
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" t="s">
+        <v>71</v>
+      </c>
+      <c r="L12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" t="s">
+        <v>53</v>
+      </c>
+      <c r="P12" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>73</v>
+      </c>
+      <c r="R12" t="s">
+        <v>74</v>
+      </c>
+      <c r="S12" t="s">
+        <v>75</v>
+      </c>
+      <c r="T12" t="s">
+        <v>76</v>
+      </c>
+      <c r="U12" t="s">
+        <v>81</v>
+      </c>
+      <c r="V12" t="s">
+        <v>52</v>
+      </c>
+      <c r="W12" t="s">
+        <v>51</v>
+      </c>
+      <c r="X12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>141</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>144</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>140</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>141</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>155</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>150</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>151</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>152</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>130</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>153</v>
+      </c>
+      <c r="BC12" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD12" t="s">
+        <v>163</v>
+      </c>
+      <c r="BE12" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="13" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1668,9 +1824,6 @@
       <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="E13" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="14" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1679,264 +1832,6 @@
       <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" t="s">
-        <v>72</v>
-      </c>
-      <c r="L14" t="s">
-        <v>73</v>
-      </c>
-      <c r="M14" t="s">
-        <v>74</v>
-      </c>
-      <c r="N14" t="s">
-        <v>60</v>
-      </c>
-      <c r="O14" t="s">
-        <v>61</v>
-      </c>
-      <c r="P14" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>64</v>
-      </c>
-      <c r="R14" t="s">
-        <v>84</v>
-      </c>
-      <c r="S14" t="s">
-        <v>62</v>
-      </c>
-      <c r="T14" t="s">
-        <v>85</v>
-      </c>
-      <c r="U14" t="s">
-        <v>86</v>
-      </c>
-      <c r="V14" t="s">
-        <v>87</v>
-      </c>
-      <c r="W14" t="s">
-        <v>83</v>
-      </c>
-      <c r="X14" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>93</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>95</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>96</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>97</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>98</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>99</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>100</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>102</v>
-      </c>
-      <c r="AM14" t="s">
-        <v>103</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>104</v>
-      </c>
-      <c r="AO14" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP14" t="s">
-        <v>88</v>
-      </c>
-      <c r="AQ14" t="s">
-        <v>89</v>
-      </c>
-      <c r="AR14" t="s">
-        <v>90</v>
-      </c>
-      <c r="AS14" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT14" t="s">
-        <v>92</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV14" t="s">
-        <v>124</v>
-      </c>
-      <c r="AW14" t="s">
-        <v>125</v>
-      </c>
-      <c r="AX14" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY14" t="s">
-        <v>83</v>
-      </c>
-      <c r="AZ14" t="s">
-        <v>88</v>
-      </c>
-      <c r="BA14" t="s">
-        <v>89</v>
-      </c>
-      <c r="BB14" t="s">
-        <v>90</v>
-      </c>
-      <c r="BC14" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD14" t="s">
-        <v>92</v>
-      </c>
-      <c r="BE14" t="s">
-        <v>93</v>
-      </c>
-      <c r="BF14" t="s">
-        <v>130</v>
-      </c>
-      <c r="BG14" t="s">
-        <v>63</v>
-      </c>
-      <c r="BH14" t="s">
-        <v>143</v>
-      </c>
-      <c r="BI14" t="s">
-        <v>137</v>
-      </c>
-      <c r="BJ14" t="s">
-        <v>139</v>
-      </c>
-      <c r="BK14" t="s">
-        <v>72</v>
-      </c>
-      <c r="BL14" t="s">
-        <v>145</v>
-      </c>
-      <c r="BM14" t="s">
-        <v>73</v>
-      </c>
-      <c r="BN14" t="s">
-        <v>146</v>
-      </c>
-      <c r="BO14" t="s">
-        <v>84</v>
-      </c>
-      <c r="BP14" t="s">
-        <v>127</v>
-      </c>
-      <c r="BQ14" t="s">
-        <v>142</v>
-      </c>
-      <c r="BR14" t="s">
-        <v>147</v>
-      </c>
-      <c r="BS14" t="s">
-        <v>149</v>
-      </c>
-      <c r="BT14" t="s">
-        <v>155</v>
-      </c>
-      <c r="BU14" t="s">
-        <v>150</v>
-      </c>
-      <c r="BV14" t="s">
-        <v>151</v>
-      </c>
-      <c r="BW14" t="s">
-        <v>130</v>
-      </c>
-      <c r="BX14" t="s">
-        <v>72</v>
-      </c>
-      <c r="BY14" t="s">
-        <v>154</v>
-      </c>
-      <c r="BZ14" t="s">
-        <v>156</v>
-      </c>
-      <c r="CA14" t="s">
-        <v>160</v>
-      </c>
-      <c r="CB14" t="s">
-        <v>157</v>
-      </c>
-      <c r="CC14" t="s">
-        <v>158</v>
-      </c>
-      <c r="CD14" t="s">
-        <v>159</v>
-      </c>
-      <c r="CE14" t="s">
-        <v>161</v>
-      </c>
-      <c r="CF14" t="s">
-        <v>165</v>
-      </c>
-      <c r="CG14" t="s">
-        <v>84</v>
-      </c>
-      <c r="CH14" t="s">
-        <v>166</v>
-      </c>
-      <c r="CI14" t="s">
-        <v>167</v>
-      </c>
-      <c r="CJ14" t="s">
-        <v>63</v>
-      </c>
-      <c r="CK14" t="s">
-        <v>168</v>
-      </c>
-      <c r="CL14" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="15" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1946,262 +1841,7 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" t="s">
-        <v>82</v>
-      </c>
-      <c r="H15" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" t="s">
-        <v>72</v>
-      </c>
-      <c r="L15" t="s">
-        <v>73</v>
-      </c>
-      <c r="M15" t="s">
-        <v>74</v>
-      </c>
-      <c r="N15" t="s">
-        <v>60</v>
-      </c>
-      <c r="O15" t="s">
-        <v>61</v>
-      </c>
-      <c r="P15" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>71</v>
-      </c>
-      <c r="R15" t="s">
-        <v>71</v>
-      </c>
-      <c r="S15" t="s">
-        <v>69</v>
-      </c>
-      <c r="T15" t="s">
-        <v>69</v>
-      </c>
-      <c r="U15" t="s">
-        <v>75</v>
-      </c>
-      <c r="V15" t="s">
-        <v>75</v>
-      </c>
-      <c r="W15" t="s">
-        <v>70</v>
-      </c>
-      <c r="X15" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AP15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AQ15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AR15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AS15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AT15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AV15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AW15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AX15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AY15" t="s">
-        <v>123</v>
-      </c>
-      <c r="AZ15" t="s">
-        <v>123</v>
-      </c>
-      <c r="BA15" t="s">
-        <v>123</v>
-      </c>
-      <c r="BB15" t="s">
-        <v>123</v>
-      </c>
-      <c r="BC15" t="s">
-        <v>123</v>
-      </c>
-      <c r="BD15" t="s">
-        <v>123</v>
-      </c>
-      <c r="BE15" t="s">
-        <v>123</v>
-      </c>
-      <c r="BF15" t="s">
-        <v>129</v>
-      </c>
-      <c r="BG15" t="s">
-        <v>129</v>
-      </c>
-      <c r="BH15" t="s">
-        <v>144</v>
-      </c>
-      <c r="BI15" t="s">
-        <v>144</v>
-      </c>
-      <c r="BJ15" t="s">
-        <v>144</v>
-      </c>
-      <c r="BK15" t="s">
-        <v>140</v>
-      </c>
-      <c r="BL15" t="s">
-        <v>140</v>
-      </c>
-      <c r="BM15" t="s">
-        <v>141</v>
-      </c>
-      <c r="BN15" t="s">
-        <v>141</v>
-      </c>
-      <c r="BO15" t="s">
-        <v>84</v>
-      </c>
-      <c r="BP15" t="s">
-        <v>127</v>
-      </c>
-      <c r="BQ15" t="s">
-        <v>142</v>
-      </c>
-      <c r="BR15" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="BS15" t="s">
-        <v>149</v>
-      </c>
-      <c r="BT15" t="s">
-        <v>155</v>
-      </c>
-      <c r="BU15" t="s">
-        <v>150</v>
-      </c>
-      <c r="BV15" t="s">
-        <v>151</v>
-      </c>
-      <c r="BW15" t="s">
-        <v>130</v>
-      </c>
-      <c r="BX15" t="s">
-        <v>153</v>
-      </c>
-      <c r="BY15" t="s">
-        <v>153</v>
-      </c>
-      <c r="BZ15" t="s">
-        <v>152</v>
-      </c>
-      <c r="CA15" t="s">
-        <v>152</v>
-      </c>
-      <c r="CB15" t="s">
-        <v>152</v>
-      </c>
-      <c r="CC15" t="s">
-        <v>152</v>
-      </c>
-      <c r="CD15" t="s">
-        <v>152</v>
-      </c>
-      <c r="CE15" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="CF15" t="s">
-        <v>163</v>
-      </c>
-      <c r="CG15" t="s">
-        <v>163</v>
-      </c>
-      <c r="CH15" t="s">
-        <v>164</v>
-      </c>
-      <c r="CI15" t="s">
-        <v>164</v>
-      </c>
-      <c r="CJ15" t="s">
-        <v>164</v>
-      </c>
-      <c r="CK15" t="s">
-        <v>164</v>
-      </c>
-      <c r="CL15" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:90" x14ac:dyDescent="0.2">
@@ -2214,775 +1854,1293 @@
       <c r="C16" t="s">
         <v>176</v>
       </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" t="s">
+        <v>72</v>
+      </c>
+      <c r="L16" t="s">
+        <v>73</v>
+      </c>
+      <c r="M16" t="s">
+        <v>74</v>
+      </c>
+      <c r="N16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O16" t="s">
+        <v>61</v>
+      </c>
+      <c r="P16" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>64</v>
+      </c>
+      <c r="R16" t="s">
+        <v>84</v>
+      </c>
+      <c r="S16" t="s">
+        <v>62</v>
+      </c>
+      <c r="T16" t="s">
+        <v>85</v>
+      </c>
+      <c r="U16" t="s">
+        <v>86</v>
+      </c>
+      <c r="V16" t="s">
+        <v>87</v>
+      </c>
+      <c r="W16" t="s">
+        <v>83</v>
+      </c>
+      <c r="X16" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>96</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>103</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV16" t="s">
+        <v>124</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>125</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>83</v>
+      </c>
+      <c r="AZ16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BA16" t="s">
+        <v>89</v>
+      </c>
+      <c r="BB16" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC16" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD16" t="s">
+        <v>92</v>
+      </c>
+      <c r="BE16" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF16" t="s">
+        <v>130</v>
+      </c>
+      <c r="BG16" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH16" t="s">
+        <v>143</v>
+      </c>
+      <c r="BI16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BJ16" t="s">
+        <v>139</v>
+      </c>
+      <c r="BK16" t="s">
+        <v>72</v>
+      </c>
+      <c r="BL16" t="s">
+        <v>145</v>
+      </c>
+      <c r="BM16" t="s">
+        <v>73</v>
+      </c>
+      <c r="BN16" t="s">
+        <v>146</v>
+      </c>
+      <c r="BO16" t="s">
+        <v>84</v>
+      </c>
+      <c r="BP16" t="s">
+        <v>127</v>
+      </c>
+      <c r="BQ16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BR16" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS16" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT16" t="s">
+        <v>155</v>
+      </c>
+      <c r="BU16" t="s">
+        <v>150</v>
+      </c>
+      <c r="BV16" t="s">
+        <v>151</v>
+      </c>
+      <c r="BW16" t="s">
+        <v>130</v>
+      </c>
+      <c r="BX16" t="s">
+        <v>72</v>
+      </c>
+      <c r="BY16" t="s">
+        <v>154</v>
+      </c>
+      <c r="BZ16" t="s">
+        <v>156</v>
+      </c>
+      <c r="CA16" t="s">
+        <v>160</v>
+      </c>
+      <c r="CB16" t="s">
+        <v>157</v>
+      </c>
+      <c r="CC16" t="s">
+        <v>158</v>
+      </c>
+      <c r="CD16" t="s">
+        <v>159</v>
+      </c>
+      <c r="CE16" t="s">
+        <v>161</v>
+      </c>
+      <c r="CF16" t="s">
+        <v>165</v>
+      </c>
+      <c r="CG16" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH16" t="s">
+        <v>166</v>
+      </c>
+      <c r="CI16" t="s">
+        <v>167</v>
+      </c>
+      <c r="CJ16" t="s">
+        <v>63</v>
+      </c>
+      <c r="CK16" t="s">
+        <v>168</v>
+      </c>
+      <c r="CL16" t="s">
+        <v>169</v>
+      </c>
     </row>
-    <row r="17" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:90" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>28</v>
+        <v>79</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" t="s">
+        <v>72</v>
+      </c>
+      <c r="L17" t="s">
+        <v>73</v>
+      </c>
+      <c r="M17" t="s">
+        <v>74</v>
+      </c>
+      <c r="N17" t="s">
+        <v>60</v>
+      </c>
+      <c r="O17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P17" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>71</v>
+      </c>
+      <c r="R17" t="s">
+        <v>71</v>
+      </c>
+      <c r="S17" t="s">
+        <v>69</v>
+      </c>
+      <c r="T17" t="s">
+        <v>69</v>
+      </c>
+      <c r="U17" t="s">
+        <v>75</v>
+      </c>
+      <c r="V17" t="s">
+        <v>75</v>
+      </c>
+      <c r="W17" t="s">
+        <v>70</v>
+      </c>
+      <c r="X17" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AV17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>123</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>123</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>123</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>123</v>
+      </c>
+      <c r="BC17" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD17" t="s">
+        <v>123</v>
+      </c>
+      <c r="BE17" t="s">
+        <v>123</v>
+      </c>
+      <c r="BF17" t="s">
+        <v>129</v>
+      </c>
+      <c r="BG17" t="s">
+        <v>129</v>
+      </c>
+      <c r="BH17" t="s">
+        <v>144</v>
+      </c>
+      <c r="BI17" t="s">
+        <v>144</v>
+      </c>
+      <c r="BJ17" t="s">
+        <v>144</v>
+      </c>
+      <c r="BK17" t="s">
+        <v>140</v>
+      </c>
+      <c r="BL17" t="s">
+        <v>140</v>
+      </c>
+      <c r="BM17" t="s">
+        <v>141</v>
+      </c>
+      <c r="BN17" t="s">
+        <v>141</v>
+      </c>
+      <c r="BO17" t="s">
+        <v>84</v>
+      </c>
+      <c r="BP17" t="s">
+        <v>127</v>
+      </c>
+      <c r="BQ17" t="s">
+        <v>142</v>
+      </c>
+      <c r="BR17" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="BS17" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BU17" t="s">
+        <v>150</v>
+      </c>
+      <c r="BV17" t="s">
+        <v>151</v>
+      </c>
+      <c r="BW17" t="s">
+        <v>130</v>
+      </c>
+      <c r="BX17" t="s">
+        <v>153</v>
+      </c>
+      <c r="BY17" t="s">
+        <v>153</v>
+      </c>
+      <c r="BZ17" t="s">
+        <v>152</v>
+      </c>
+      <c r="CA17" t="s">
+        <v>152</v>
+      </c>
+      <c r="CB17" t="s">
+        <v>152</v>
+      </c>
+      <c r="CC17" t="s">
+        <v>152</v>
+      </c>
+      <c r="CD17" t="s">
+        <v>152</v>
+      </c>
+      <c r="CE17" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="CF17" t="s">
+        <v>163</v>
+      </c>
+      <c r="CG17" t="s">
+        <v>163</v>
+      </c>
+      <c r="CH17" t="s">
+        <v>164</v>
+      </c>
+      <c r="CI17" t="s">
+        <v>164</v>
+      </c>
+      <c r="CJ17" t="s">
+        <v>164</v>
+      </c>
+      <c r="CK17" t="s">
+        <v>164</v>
+      </c>
+      <c r="CL17" t="s">
+        <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E18" t="s">
+    </row>
+    <row r="19" spans="1:90" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:90" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
         <v>111</v>
       </c>
-      <c r="F18" t="str">
+      <c r="F20" t="str">
         <f>H30</f>
         <v>Comp 401</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G20" t="s">
         <v>52</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H20" t="s">
         <v>51</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I20" t="s">
         <v>53</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J20" t="s">
         <v>72</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K20" t="s">
         <v>73</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L20" t="s">
         <v>74</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M20" t="s">
         <v>60</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N20" t="s">
         <v>60</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O20" t="s">
         <v>60</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P20" t="s">
         <v>61</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="Q20" t="s">
         <v>61</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R20" t="s">
         <v>61</v>
       </c>
-      <c r="S18" t="s">
+      <c r="S20" t="s">
         <v>63</v>
       </c>
-      <c r="T18" t="s">
+      <c r="T20" t="s">
         <v>64</v>
       </c>
-      <c r="U18" t="s">
+      <c r="U20" t="s">
         <v>84</v>
       </c>
-      <c r="V18" t="s">
+      <c r="V20" t="s">
         <v>62</v>
       </c>
-      <c r="W18" t="s">
+      <c r="W20" t="s">
         <v>85</v>
       </c>
-      <c r="X18" t="s">
+      <c r="X20" t="s">
         <v>85</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Y20" t="s">
         <v>86</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="Z20" t="s">
         <v>86</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AA20" t="s">
         <v>87</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AB20" t="s">
         <v>87</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AC20" t="s">
         <v>83</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AD20" t="s">
         <v>83</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AE20" t="s">
         <v>88</v>
       </c>
-      <c r="AF18" t="s">
+      <c r="AF20" t="s">
         <v>88</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AG20" t="s">
         <v>89</v>
       </c>
-      <c r="AH18" t="s">
+      <c r="AH20" t="s">
         <v>89</v>
       </c>
-      <c r="AI18" t="s">
+      <c r="AI20" t="s">
         <v>90</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AJ20" t="s">
         <v>90</v>
       </c>
-      <c r="AK18" t="s">
+      <c r="AK20" t="s">
         <v>91</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AL20" t="s">
         <v>91</v>
       </c>
-      <c r="AM18" t="s">
+      <c r="AM20" t="s">
         <v>92</v>
       </c>
-      <c r="AN18" t="s">
+      <c r="AN20" t="s">
         <v>93</v>
       </c>
-      <c r="AO18" t="s">
+      <c r="AO20" t="s">
         <v>96</v>
       </c>
-      <c r="AP18" t="s">
+      <c r="AP20" t="s">
         <v>97</v>
       </c>
-      <c r="AQ18" t="s">
+      <c r="AQ20" t="s">
         <v>99</v>
       </c>
-      <c r="AR18" t="s">
+      <c r="AR20" t="s">
         <v>101</v>
       </c>
-      <c r="AS18" t="s">
+      <c r="AS20" t="s">
         <v>101</v>
       </c>
-      <c r="AT18" t="s">
+      <c r="AT20" t="s">
         <v>102</v>
       </c>
-      <c r="AU18" t="s">
+      <c r="AU20" t="s">
         <v>102</v>
       </c>
-      <c r="AV18" t="s">
+      <c r="AV20" t="s">
         <v>103</v>
       </c>
-      <c r="AW18" t="s">
+      <c r="AW20" t="s">
         <v>103</v>
       </c>
-      <c r="AX18" t="s">
+      <c r="AX20" t="s">
         <v>126</v>
       </c>
-      <c r="AY18" t="s">
+      <c r="AY20" t="s">
         <v>126</v>
       </c>
-      <c r="AZ18" t="s">
+      <c r="AZ20" t="s">
         <v>104</v>
       </c>
-      <c r="BA18" t="s">
+      <c r="BA20" t="s">
         <v>125</v>
       </c>
-      <c r="BB18" t="s">
+      <c r="BB20" t="s">
         <v>127</v>
       </c>
-      <c r="BC18" t="s">
+      <c r="BC20" t="s">
         <v>130</v>
       </c>
-      <c r="BD18" t="s">
+      <c r="BD20" t="s">
         <v>63</v>
       </c>
-      <c r="BE18" t="s">
+      <c r="BE20" t="s">
         <v>136</v>
       </c>
-      <c r="BF18" t="s">
+      <c r="BF20" t="s">
         <v>143</v>
       </c>
-      <c r="BG18" t="s">
+      <c r="BG20" t="s">
         <v>137</v>
       </c>
-      <c r="BH18" t="s">
+      <c r="BH20" t="s">
         <v>139</v>
       </c>
-      <c r="BI18" t="s">
+      <c r="BI20" t="s">
         <v>145</v>
       </c>
-      <c r="BJ18" t="s">
+      <c r="BJ20" t="s">
         <v>146</v>
       </c>
-      <c r="BK18" t="s">
+      <c r="BK20" t="s">
         <v>146</v>
       </c>
-      <c r="BL18" t="s">
+      <c r="BL20" t="s">
         <v>142</v>
       </c>
-      <c r="BM18" t="s">
+      <c r="BM20" t="s">
         <v>182</v>
       </c>
-      <c r="BN18" t="s">
+      <c r="BN20" t="s">
         <v>147</v>
       </c>
-      <c r="BO18" t="s">
+      <c r="BO20" t="s">
         <v>155</v>
       </c>
-      <c r="BP18" t="s">
+      <c r="BP20" t="s">
         <v>150</v>
       </c>
-      <c r="BQ18" t="s">
+      <c r="BQ20" t="s">
         <v>150</v>
       </c>
-      <c r="BR18" t="s">
+      <c r="BR20" t="s">
         <v>150</v>
       </c>
-      <c r="BS18" t="s">
+      <c r="BS20" t="s">
         <v>151</v>
       </c>
-      <c r="BT18" t="s">
+      <c r="BT20" t="s">
         <v>154</v>
       </c>
-      <c r="BU18" t="s">
+      <c r="BU20" t="s">
         <v>156</v>
       </c>
-      <c r="BV18" t="s">
+      <c r="BV20" t="s">
         <v>160</v>
       </c>
-      <c r="BW18" t="s">
+      <c r="BW20" t="s">
         <v>157</v>
       </c>
-      <c r="BX18" t="s">
+      <c r="BX20" t="s">
         <v>157</v>
       </c>
-      <c r="BY18" t="s">
+      <c r="BY20" t="s">
         <v>158</v>
       </c>
-      <c r="BZ18" t="s">
+      <c r="BZ20" t="s">
         <v>159</v>
       </c>
-      <c r="CA18" t="s">
+      <c r="CA20" t="s">
         <v>161</v>
       </c>
-      <c r="CB18" t="s">
+      <c r="CB20" t="s">
         <v>165</v>
       </c>
-      <c r="CC18" t="s">
+      <c r="CC20" t="s">
         <v>166</v>
       </c>
-      <c r="CD18" t="s">
+      <c r="CD20" t="s">
         <v>167</v>
       </c>
-      <c r="CE18" t="s">
+      <c r="CE20" t="s">
         <v>63</v>
       </c>
-      <c r="CF18" t="s">
+      <c r="CF20" t="s">
         <v>168</v>
       </c>
-      <c r="CG18" t="s">
+      <c r="CG20" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
+    <row r="21" spans="1:90" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
         <v>112</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>50</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G21" t="s">
         <v>80</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H21" t="s">
         <v>52</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I21" t="s">
         <v>52</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J21" t="s">
         <v>136</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K21" t="s">
         <v>72</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L21" t="s">
         <v>73</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M21" t="s">
         <v>52</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N21" t="s">
         <v>64</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O21" t="s">
         <v>84</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P21" t="s">
         <v>51</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="Q21" t="s">
         <v>64</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R21" t="s">
         <v>84</v>
       </c>
-      <c r="S19" t="s">
+      <c r="S21" t="s">
         <v>74</v>
       </c>
-      <c r="T19" t="s">
+      <c r="T21" t="s">
         <v>72</v>
       </c>
-      <c r="U19" t="s">
+      <c r="U21" t="s">
         <v>73</v>
       </c>
-      <c r="V19" t="s">
+      <c r="V21" t="s">
         <v>74</v>
       </c>
-      <c r="W19" t="s">
+      <c r="W21" t="s">
         <v>84</v>
       </c>
-      <c r="X19" t="s">
+      <c r="X21" t="s">
         <v>127</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Y21" t="s">
         <v>72</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="Z21" t="s">
         <v>73</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AA21" t="s">
         <v>73</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AB21" t="s">
         <v>72</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AC21" t="s">
         <v>53</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AD21" t="s">
         <v>51</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AE21" t="s">
         <v>53</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AF21" t="s">
         <v>51</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AG21" t="s">
         <v>53</v>
       </c>
-      <c r="AH19" t="s">
+      <c r="AH21" t="s">
         <v>51</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AI21" t="s">
         <v>53</v>
       </c>
-      <c r="AJ19" t="s">
+      <c r="AJ21" t="s">
         <v>51</v>
       </c>
-      <c r="AK19" t="s">
+      <c r="AK21" t="s">
         <v>53</v>
       </c>
-      <c r="AL19" t="s">
+      <c r="AL21" t="s">
         <v>51</v>
       </c>
-      <c r="AM19" t="s">
+      <c r="AM21" t="s">
         <v>51</v>
       </c>
-      <c r="AN19" t="s">
+      <c r="AN21" t="s">
         <v>51</v>
       </c>
-      <c r="AO19" t="s">
+      <c r="AO21" t="s">
         <v>95</v>
       </c>
-      <c r="AP19" t="s">
+      <c r="AP21" t="s">
         <v>96</v>
       </c>
-      <c r="AQ19" t="s">
+      <c r="AQ21" t="s">
         <v>98</v>
       </c>
-      <c r="AR19" t="s">
+      <c r="AR21" t="s">
         <v>73</v>
       </c>
-      <c r="AS19" t="s">
+      <c r="AS21" t="s">
         <v>86</v>
       </c>
-      <c r="AT19" t="s">
+      <c r="AT21" t="s">
         <v>113</v>
       </c>
-      <c r="AU19" t="s">
+      <c r="AU21" t="s">
         <v>87</v>
       </c>
-      <c r="AV19" t="s">
+      <c r="AV21" t="s">
         <v>114</v>
       </c>
-      <c r="AW19" t="s">
+      <c r="AW21" t="s">
         <v>102</v>
       </c>
-      <c r="AX19" t="s">
+      <c r="AX21" t="s">
         <v>128</v>
       </c>
-      <c r="AY19" t="s">
+      <c r="AY21" t="s">
         <v>87</v>
       </c>
-      <c r="AZ19" t="s">
+      <c r="AZ21" t="s">
         <v>103</v>
       </c>
-      <c r="BA19" t="s">
+      <c r="BA21" t="s">
         <v>127</v>
       </c>
-      <c r="BB19" t="s">
+      <c r="BB21" t="s">
         <v>74</v>
       </c>
-      <c r="BC19" t="s">
+      <c r="BC21" t="s">
         <v>131</v>
       </c>
-      <c r="BD19" t="s">
+      <c r="BD21" t="s">
         <v>74</v>
       </c>
-      <c r="BE19" t="s">
+      <c r="BE21" t="s">
         <v>131</v>
       </c>
-      <c r="BF19" t="s">
+      <c r="BF21" t="s">
         <v>127</v>
       </c>
-      <c r="BG19" t="s">
+      <c r="BG21" t="s">
         <v>127</v>
       </c>
-      <c r="BH19" t="s">
+      <c r="BH21" t="s">
         <v>127</v>
       </c>
-      <c r="BI19" t="s">
+      <c r="BI21" t="s">
         <v>136</v>
       </c>
-      <c r="BJ19" t="s">
+      <c r="BJ21" t="s">
         <v>145</v>
       </c>
-      <c r="BK19" t="s">
+      <c r="BK21" t="s">
         <v>72</v>
       </c>
-      <c r="BL19" t="s">
+      <c r="BL21" t="s">
         <v>74</v>
       </c>
-      <c r="BM19" t="s">
+      <c r="BM21" t="s">
         <v>84</v>
       </c>
-      <c r="BN19" t="s">
+      <c r="BN21" t="s">
         <v>84</v>
       </c>
-      <c r="BO19" t="s">
+      <c r="BO21" t="s">
         <v>149</v>
       </c>
-      <c r="BP19" t="s">
+      <c r="BP21" t="s">
         <v>149</v>
       </c>
-      <c r="BQ19" t="s">
+      <c r="BQ21" t="s">
         <v>72</v>
       </c>
-      <c r="BR19" t="s">
+      <c r="BR21" t="s">
         <v>154</v>
       </c>
-      <c r="BS19" t="s">
+      <c r="BS21" t="s">
         <v>150</v>
       </c>
-      <c r="BT19" t="s">
+      <c r="BT21" t="s">
         <v>131</v>
       </c>
-      <c r="BU19" t="s">
+      <c r="BU21" t="s">
         <v>151</v>
       </c>
-      <c r="BV19" t="s">
+      <c r="BV21" t="s">
         <v>150</v>
       </c>
-      <c r="BW19" t="s">
+      <c r="BW21" t="s">
         <v>150</v>
       </c>
-      <c r="BX19" t="s">
+      <c r="BX21" t="s">
         <v>74</v>
       </c>
-      <c r="BY19" t="s">
+      <c r="BY21" t="s">
         <v>160</v>
       </c>
-      <c r="BZ19" t="s">
+      <c r="BZ21" t="s">
         <v>161</v>
       </c>
-      <c r="CA19" t="s">
+      <c r="CA21" t="s">
         <v>150</v>
       </c>
-      <c r="CB19" t="s">
+      <c r="CB21" t="s">
         <v>131</v>
       </c>
-      <c r="CC19" t="s">
+      <c r="CC21" t="s">
         <v>130</v>
       </c>
-      <c r="CD19" t="s">
+      <c r="CD21" t="s">
         <v>62</v>
       </c>
-      <c r="CE19" t="s">
+      <c r="CE21" t="s">
         <v>74</v>
       </c>
-      <c r="CF19" t="s">
+      <c r="CF21" t="s">
         <v>63</v>
       </c>
-      <c r="CG19" t="s">
+      <c r="CG21" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" t="s">
-        <v>178</v>
-      </c>
-      <c r="G20" t="s">
-        <v>178</v>
-      </c>
-      <c r="H20" t="s">
-        <v>177</v>
-      </c>
-      <c r="I20" t="s">
-        <v>177</v>
-      </c>
-      <c r="J20" t="s">
-        <v>177</v>
-      </c>
-      <c r="K20" t="s">
-        <v>177</v>
-      </c>
-      <c r="L20" t="s">
-        <v>177</v>
-      </c>
-      <c r="M20" t="s">
-        <v>177</v>
-      </c>
-      <c r="N20" t="s">
-        <v>179</v>
-      </c>
-      <c r="O20" t="s">
-        <v>179</v>
-      </c>
-      <c r="P20" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>179</v>
-      </c>
-      <c r="R20" t="s">
-        <v>179</v>
-      </c>
-      <c r="S20" t="s">
-        <v>177</v>
-      </c>
-      <c r="T20" t="s">
-        <v>177</v>
-      </c>
-      <c r="U20" t="s">
-        <v>177</v>
-      </c>
-      <c r="V20" t="s">
-        <v>177</v>
-      </c>
-      <c r="W20" t="s">
-        <v>177</v>
-      </c>
-      <c r="X20" t="s">
-        <v>177</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AJ20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AK20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AL20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AM20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AO20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AP20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AQ20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AR20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AS20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AT20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AU20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AV20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AW20" t="s">
-        <v>177</v>
-      </c>
-      <c r="AX20" t="s">
-        <v>180</v>
-      </c>
-      <c r="AY20" t="s">
-        <v>180</v>
-      </c>
-      <c r="AZ20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BA20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BB20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BC20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BD20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BE20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BF20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BG20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BH20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BI20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BJ20" t="s">
-        <v>181</v>
-      </c>
-      <c r="BK20" t="s">
-        <v>181</v>
-      </c>
-      <c r="BL20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BM20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BN20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BO20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BP20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BQ20" t="s">
-        <v>183</v>
-      </c>
-      <c r="BR20" t="s">
-        <v>183</v>
-      </c>
-      <c r="BS20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BT20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BU20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BV20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BW20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BX20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BY20" t="s">
-        <v>177</v>
-      </c>
-      <c r="BZ20" t="s">
-        <v>177</v>
-      </c>
-      <c r="CA20" t="s">
-        <v>177</v>
-      </c>
-      <c r="CB20" t="s">
-        <v>177</v>
-      </c>
-      <c r="CC20" t="s">
-        <v>177</v>
-      </c>
-      <c r="CD20" t="s">
-        <v>177</v>
-      </c>
-      <c r="CE20" t="s">
-        <v>177</v>
-      </c>
-      <c r="CF20" t="s">
-        <v>177</v>
-      </c>
-      <c r="CG20" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" t="s">
+        <v>178</v>
+      </c>
+      <c r="H22" t="s">
+        <v>177</v>
+      </c>
+      <c r="I22" t="s">
+        <v>177</v>
+      </c>
+      <c r="J22" t="s">
+        <v>177</v>
+      </c>
+      <c r="K22" t="s">
+        <v>177</v>
+      </c>
+      <c r="L22" t="s">
+        <v>177</v>
+      </c>
+      <c r="M22" t="s">
+        <v>177</v>
+      </c>
+      <c r="N22" t="s">
+        <v>179</v>
+      </c>
+      <c r="O22" t="s">
+        <v>179</v>
+      </c>
+      <c r="P22" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>179</v>
+      </c>
+      <c r="R22" t="s">
+        <v>179</v>
+      </c>
+      <c r="S22" t="s">
+        <v>177</v>
+      </c>
+      <c r="T22" t="s">
+        <v>177</v>
+      </c>
+      <c r="U22" t="s">
+        <v>177</v>
+      </c>
+      <c r="V22" t="s">
+        <v>177</v>
+      </c>
+      <c r="W22" t="s">
+        <v>177</v>
+      </c>
+      <c r="X22" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AW22" t="s">
+        <v>177</v>
+      </c>
+      <c r="AX22" t="s">
+        <v>180</v>
+      </c>
+      <c r="AY22" t="s">
+        <v>180</v>
+      </c>
+      <c r="AZ22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BA22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BB22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BC22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BD22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BE22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BF22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BG22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BH22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BJ22" t="s">
+        <v>181</v>
+      </c>
+      <c r="BK22" t="s">
+        <v>181</v>
+      </c>
+      <c r="BL22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BM22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BN22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BO22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BP22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BQ22" t="s">
+        <v>183</v>
+      </c>
+      <c r="BR22" t="s">
+        <v>183</v>
+      </c>
+      <c r="BS22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BT22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BU22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BV22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BW22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BX22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BY22" t="s">
+        <v>177</v>
+      </c>
+      <c r="BZ22" t="s">
+        <v>177</v>
+      </c>
+      <c r="CA22" t="s">
+        <v>177</v>
+      </c>
+      <c r="CB22" t="s">
+        <v>177</v>
+      </c>
+      <c r="CC22" t="s">
+        <v>177</v>
+      </c>
+      <c r="CD22" t="s">
+        <v>177</v>
+      </c>
+      <c r="CE22" t="s">
+        <v>177</v>
+      </c>
+      <c r="CF22" t="s">
+        <v>177</v>
+      </c>
+      <c r="CG22" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="23" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2996,7 +3154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -3004,7 +3162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -3012,7 +3170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -3020,7 +3178,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -3028,7 +3186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -3036,7 +3194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>5</v>
       </c>
@@ -3254,7 +3412,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -3466,7 +3624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
updated for final upload
adjusted to course id and program req id
</commit_message>
<xml_diff>
--- a/db_schema.xlsx
+++ b/db_schema.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="181">
   <si>
     <t>Users</t>
   </si>
@@ -646,8 +646,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -665,15 +667,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -949,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CL46"/>
+  <dimension ref="A1:DF46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="93" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="J19" sqref="F18:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -965,7 +969,7 @@
     <col min="21" max="21" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -982,7 +986,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -990,7 +994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1028,7 +1032,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1060,7 +1064,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1092,7 +1096,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1124,7 +1128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:90" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:110" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1132,7 +1136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1149,7 +1153,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1319,7 +1323,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:110" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>23</v>
       </c>
@@ -1480,7 +1484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:110" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>18</v>
       </c>
@@ -1641,7 +1645,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1802,7 +1806,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1816,7 +1820,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1824,7 +1828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1835,7 +1839,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>172</v>
       </c>
@@ -2103,8 +2107,68 @@
       <c r="CL16">
         <v>67</v>
       </c>
+      <c r="CM16">
+        <v>44</v>
+      </c>
+      <c r="CN16">
+        <v>45</v>
+      </c>
+      <c r="CO16">
+        <v>46</v>
+      </c>
+      <c r="CP16">
+        <v>50</v>
+      </c>
+      <c r="CQ16">
+        <v>19</v>
+      </c>
+      <c r="CR16">
+        <v>47</v>
+      </c>
+      <c r="CS16">
+        <v>20</v>
+      </c>
+      <c r="CT16">
+        <v>48</v>
+      </c>
+      <c r="CU16">
+        <v>22</v>
+      </c>
+      <c r="CV16">
+        <v>40</v>
+      </c>
+      <c r="CW16">
+        <v>41</v>
+      </c>
+      <c r="CX16">
+        <v>10</v>
+      </c>
+      <c r="CY16">
+        <v>22</v>
+      </c>
+      <c r="CZ16">
+        <v>8</v>
+      </c>
+      <c r="DA16">
+        <v>18</v>
+      </c>
+      <c r="DB16">
+        <v>1</v>
+      </c>
+      <c r="DC16">
+        <v>2</v>
+      </c>
+      <c r="DD16">
+        <v>1</v>
+      </c>
+      <c r="DE16">
+        <v>2</v>
+      </c>
+      <c r="DF16">
+        <v>21</v>
+      </c>
     </row>
-    <row r="17" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:110" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>79</v>
       </c>
@@ -2126,265 +2190,310 @@
       <c r="K17">
         <v>11</v>
       </c>
-      <c r="L17" t="s">
-        <v>73</v>
-      </c>
-      <c r="M17" t="s">
-        <v>74</v>
-      </c>
-      <c r="N17" t="s">
-        <v>60</v>
-      </c>
-      <c r="O17" t="s">
-        <v>61</v>
-      </c>
-      <c r="P17" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>71</v>
-      </c>
-      <c r="R17" t="s">
-        <v>71</v>
-      </c>
-      <c r="S17" t="s">
-        <v>69</v>
-      </c>
-      <c r="T17" t="s">
-        <v>69</v>
-      </c>
-      <c r="U17" t="s">
-        <v>75</v>
-      </c>
-      <c r="V17" t="s">
-        <v>75</v>
-      </c>
-      <c r="W17" t="s">
-        <v>70</v>
-      </c>
-      <c r="X17" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AP17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AQ17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AR17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AS17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AT17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AU17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AV17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AW17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AX17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AY17" t="s">
-        <v>121</v>
-      </c>
-      <c r="AZ17" t="s">
-        <v>121</v>
-      </c>
-      <c r="BA17" t="s">
-        <v>121</v>
-      </c>
-      <c r="BB17" t="s">
-        <v>121</v>
-      </c>
-      <c r="BC17" t="s">
-        <v>121</v>
-      </c>
-      <c r="BD17" t="s">
-        <v>121</v>
-      </c>
-      <c r="BE17" t="s">
-        <v>121</v>
-      </c>
-      <c r="BF17" t="s">
-        <v>126</v>
-      </c>
-      <c r="BG17" t="s">
-        <v>126</v>
-      </c>
-      <c r="BH17" t="s">
-        <v>141</v>
-      </c>
-      <c r="BI17" t="s">
-        <v>141</v>
-      </c>
-      <c r="BJ17" t="s">
-        <v>141</v>
-      </c>
-      <c r="BK17" t="s">
-        <v>137</v>
-      </c>
-      <c r="BL17" t="s">
-        <v>137</v>
-      </c>
-      <c r="BM17" t="s">
-        <v>138</v>
-      </c>
-      <c r="BN17" t="s">
-        <v>138</v>
-      </c>
-      <c r="BO17" t="s">
-        <v>83</v>
-      </c>
-      <c r="BP17" t="s">
-        <v>125</v>
-      </c>
-      <c r="BQ17" t="s">
-        <v>139</v>
-      </c>
-      <c r="BR17" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="BS17" t="s">
-        <v>146</v>
-      </c>
-      <c r="BT17" t="s">
-        <v>152</v>
-      </c>
-      <c r="BU17" t="s">
-        <v>147</v>
-      </c>
-      <c r="BV17" t="s">
-        <v>148</v>
-      </c>
-      <c r="BW17" t="s">
-        <v>127</v>
-      </c>
-      <c r="BX17" t="s">
-        <v>150</v>
-      </c>
-      <c r="BY17" t="s">
-        <v>150</v>
-      </c>
-      <c r="BZ17" t="s">
-        <v>149</v>
-      </c>
-      <c r="CA17" t="s">
-        <v>149</v>
-      </c>
-      <c r="CB17" t="s">
-        <v>149</v>
-      </c>
-      <c r="CC17" t="s">
-        <v>149</v>
-      </c>
-      <c r="CD17" t="s">
-        <v>149</v>
-      </c>
-      <c r="CE17" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="CF17" t="s">
-        <v>160</v>
-      </c>
-      <c r="CG17" t="s">
-        <v>160</v>
-      </c>
-      <c r="CH17" t="s">
-        <v>161</v>
-      </c>
-      <c r="CI17" t="s">
-        <v>161</v>
-      </c>
-      <c r="CJ17" t="s">
-        <v>161</v>
-      </c>
-      <c r="CK17" t="s">
-        <v>161</v>
-      </c>
-      <c r="CL17" t="s">
-        <v>161</v>
+      <c r="L17">
+        <v>12</v>
+      </c>
+      <c r="M17">
+        <v>13</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <v>4</v>
+      </c>
+      <c r="Q17">
+        <v>6</v>
+      </c>
+      <c r="R17">
+        <v>6</v>
+      </c>
+      <c r="S17">
+        <v>3</v>
+      </c>
+      <c r="T17">
+        <v>3</v>
+      </c>
+      <c r="U17">
+        <v>14</v>
+      </c>
+      <c r="V17">
+        <v>14</v>
+      </c>
+      <c r="W17">
+        <v>5</v>
+      </c>
+      <c r="X17">
+        <v>5</v>
+      </c>
+      <c r="Y17">
+        <v>5</v>
+      </c>
+      <c r="Z17">
+        <v>5</v>
+      </c>
+      <c r="AA17">
+        <v>5</v>
+      </c>
+      <c r="AB17">
+        <v>5</v>
+      </c>
+      <c r="AC17">
+        <v>5</v>
+      </c>
+      <c r="AD17">
+        <v>15</v>
+      </c>
+      <c r="AE17">
+        <v>15</v>
+      </c>
+      <c r="AF17">
+        <v>15</v>
+      </c>
+      <c r="AG17">
+        <v>15</v>
+      </c>
+      <c r="AH17">
+        <v>15</v>
+      </c>
+      <c r="AI17">
+        <v>15</v>
+      </c>
+      <c r="AJ17">
+        <v>15</v>
+      </c>
+      <c r="AK17">
+        <v>15</v>
+      </c>
+      <c r="AL17">
+        <v>15</v>
+      </c>
+      <c r="AM17">
+        <v>15</v>
+      </c>
+      <c r="AN17">
+        <v>15</v>
+      </c>
+      <c r="AO17">
+        <v>20</v>
+      </c>
+      <c r="AP17">
+        <v>20</v>
+      </c>
+      <c r="AQ17">
+        <v>20</v>
+      </c>
+      <c r="AR17">
+        <v>20</v>
+      </c>
+      <c r="AS17">
+        <v>20</v>
+      </c>
+      <c r="AT17">
+        <v>20</v>
+      </c>
+      <c r="AU17">
+        <v>20</v>
+      </c>
+      <c r="AV17">
+        <v>20</v>
+      </c>
+      <c r="AW17">
+        <v>20</v>
+      </c>
+      <c r="AX17">
+        <v>20</v>
+      </c>
+      <c r="AY17">
+        <v>28</v>
+      </c>
+      <c r="AZ17">
+        <v>28</v>
+      </c>
+      <c r="BA17">
+        <v>28</v>
+      </c>
+      <c r="BB17">
+        <v>28</v>
+      </c>
+      <c r="BC17">
+        <v>28</v>
+      </c>
+      <c r="BD17">
+        <v>28</v>
+      </c>
+      <c r="BE17">
+        <v>28</v>
+      </c>
+      <c r="BF17">
+        <v>23</v>
+      </c>
+      <c r="BG17">
+        <v>23</v>
+      </c>
+      <c r="BH17">
+        <v>36</v>
+      </c>
+      <c r="BI17">
+        <v>36</v>
+      </c>
+      <c r="BJ17">
+        <v>36</v>
+      </c>
+      <c r="BK17">
+        <v>29</v>
+      </c>
+      <c r="BL17">
+        <v>29</v>
+      </c>
+      <c r="BM17">
+        <v>30</v>
+      </c>
+      <c r="BN17">
+        <v>30</v>
+      </c>
+      <c r="BO17">
+        <v>32</v>
+      </c>
+      <c r="BP17">
+        <v>33</v>
+      </c>
+      <c r="BQ17">
+        <v>34</v>
+      </c>
+      <c r="BR17" s="5">
+        <v>36</v>
+      </c>
+      <c r="BS17">
+        <v>43</v>
+      </c>
+      <c r="BT17">
+        <v>44</v>
+      </c>
+      <c r="BU17">
+        <v>45</v>
+      </c>
+      <c r="BV17">
+        <v>46</v>
+      </c>
+      <c r="BW17">
+        <v>48</v>
+      </c>
+      <c r="BX17">
+        <v>49</v>
+      </c>
+      <c r="BY17">
+        <v>49</v>
+      </c>
+      <c r="BZ17">
+        <v>47</v>
+      </c>
+      <c r="CA17">
+        <v>47</v>
+      </c>
+      <c r="CB17">
+        <v>47</v>
+      </c>
+      <c r="CC17">
+        <v>47</v>
+      </c>
+      <c r="CD17">
+        <v>47</v>
+      </c>
+      <c r="CE17" s="5">
+        <v>47</v>
+      </c>
+      <c r="CF17">
+        <v>51</v>
+      </c>
+      <c r="CG17">
+        <v>51</v>
+      </c>
+      <c r="CH17">
+        <v>52</v>
+      </c>
+      <c r="CI17">
+        <v>52</v>
+      </c>
+      <c r="CJ17">
+        <v>52</v>
+      </c>
+      <c r="CK17">
+        <v>52</v>
+      </c>
+      <c r="CL17">
+        <v>52</v>
+      </c>
+      <c r="CM17">
+        <v>39</v>
+      </c>
+      <c r="CN17">
+        <v>39</v>
+      </c>
+      <c r="CO17">
+        <v>39</v>
+      </c>
+      <c r="CP17">
+        <v>39</v>
+      </c>
+      <c r="CQ17">
+        <v>40</v>
+      </c>
+      <c r="CR17">
+        <v>40</v>
+      </c>
+      <c r="CS17">
+        <v>41</v>
+      </c>
+      <c r="CT17">
+        <v>41</v>
+      </c>
+      <c r="CU17">
+        <v>37</v>
+      </c>
+      <c r="CV17">
+        <v>38</v>
+      </c>
+      <c r="CW17">
+        <v>40</v>
+      </c>
+      <c r="CX17">
+        <v>21</v>
+      </c>
+      <c r="CY17">
+        <v>21</v>
+      </c>
+      <c r="CZ17">
+        <v>35</v>
+      </c>
+      <c r="DA17">
+        <v>35</v>
+      </c>
+      <c r="DB17">
+        <v>16</v>
+      </c>
+      <c r="DC17">
+        <v>16</v>
+      </c>
+      <c r="DD17">
+        <v>24</v>
+      </c>
+      <c r="DE17">
+        <v>24</v>
+      </c>
+      <c r="DF17">
+        <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="L18">
-        <v>20</v>
-      </c>
-      <c r="M18">
-        <v>21</v>
-      </c>
-      <c r="N18">
-        <v>6</v>
-      </c>
     </row>
-    <row r="19" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2394,14 +2503,8 @@
       <c r="C19" t="s">
         <v>13</v>
       </c>
-      <c r="F19">
-        <v>16</v>
-      </c>
-      <c r="G19">
-        <v>16</v>
-      </c>
     </row>
-    <row r="20" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2411,27 +2514,13 @@
       <c r="C20" t="s">
         <v>16</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
     </row>
-    <row r="21" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="F21">
-        <v>24</v>
-      </c>
-      <c r="G21">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2445,7 +2534,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2456,7 +2545,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2708,7 +2797,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2959,7 +3048,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -3210,7 +3299,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -3419,7 +3508,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>5</v>
       </c>
@@ -3637,7 +3726,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -3849,7 +3938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>23</v>
       </c>

</xml_diff>